<commit_message>
Scale hourly constants by VOT ratio I95_xpress
use value of time ratio to scale hourly constants
</commit_message>
<xml_diff>
--- a/Analysis & Profiles/Output_2020A2.xlsx
+++ b/Analysis & Profiles/Output_2020A2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\Veterans ELToDv2.3 2017-0628\Analysis &amp; Profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\Veterans ELToDv2.3 2017-0628\Analysis &amp; Profiles\Veterans 2017-0801_newpp_revisedparams_aawdt_for_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R764"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U44" sqref="U44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,25 +1641,25 @@
         <v>15</v>
       </c>
       <c r="B6" s="30">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="C6" s="31">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D6" s="32">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E6" s="32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F6" s="33">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G6" s="84">
-        <v>6.3492063492063489E-2</v>
+        <v>0.13147410358565736</v>
       </c>
       <c r="H6" s="85">
-        <v>6.5789473684210523E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I6" s="90">
         <v>0.04</v>
@@ -1668,10 +1668,10 @@
         <v>0.01</v>
       </c>
       <c r="K6" s="92">
+        <v>0.02</v>
+      </c>
+      <c r="L6" s="93">
         <v>0.01</v>
-      </c>
-      <c r="L6" s="93">
-        <v>0</v>
       </c>
       <c r="M6" s="94">
         <v>60</v>
@@ -1697,25 +1697,25 @@
         <v>16</v>
       </c>
       <c r="B7" s="30">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C7" s="31">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="32">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E7" s="32">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F7" s="33">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G7" s="84">
-        <v>6.4285714285714279E-2</v>
+        <v>0.1357142857142857</v>
       </c>
       <c r="H7" s="85">
-        <v>7.2727272727272724E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I7" s="94">
         <v>0.02</v>
@@ -1724,7 +1724,7 @@
         <v>0.01</v>
       </c>
       <c r="K7" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L7" s="79">
         <v>0</v>
@@ -1753,34 +1753,34 @@
         <v>17</v>
       </c>
       <c r="B8" s="30">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C8" s="31">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="32">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E8" s="32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F8" s="33">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G8" s="84">
-        <v>6.3829787234042548E-2</v>
+        <v>0.1276595744680851</v>
       </c>
       <c r="H8" s="85">
-        <v>0.06</v>
+        <v>0.13725490196078433</v>
       </c>
       <c r="I8" s="94">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="J8" s="95">
         <v>0.01</v>
       </c>
       <c r="K8" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L8" s="79">
         <v>0</v>
@@ -1809,25 +1809,25 @@
         <v>18</v>
       </c>
       <c r="B9" s="30">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" s="31">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D9" s="32">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" s="32">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F9" s="33">
         <v>191</v>
       </c>
       <c r="G9" s="84">
-        <v>6.8181818181818177E-2</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="H9" s="85">
-        <v>6.7961165048543687E-2</v>
+        <v>0.13592233009708737</v>
       </c>
       <c r="I9" s="94">
         <v>0.01</v>
@@ -1836,10 +1836,10 @@
         <v>0.02</v>
       </c>
       <c r="K9" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L9" s="79">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M9" s="94">
         <v>60</v>
@@ -1865,37 +1865,37 @@
         <v>19</v>
       </c>
       <c r="B10" s="30">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C10" s="31">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="D10" s="32">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10" s="32">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F10" s="33">
         <v>406</v>
       </c>
       <c r="G10" s="84">
-        <v>6.6666666666666666E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="H10" s="85">
-        <v>6.6433566433566432E-2</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="I10" s="94">
         <v>0.02</v>
       </c>
       <c r="J10" s="95">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="K10" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L10" s="79">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M10" s="94">
         <v>60</v>
@@ -1921,37 +1921,37 @@
         <v>20</v>
       </c>
       <c r="B11" s="30">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C11" s="31">
-        <v>847</v>
+        <v>801</v>
       </c>
       <c r="D11" s="32">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E11" s="32">
-        <v>201</v>
+        <v>247</v>
       </c>
       <c r="F11" s="33">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="G11" s="84">
-        <v>0.18421052631578946</v>
+        <v>0.22707423580786026</v>
       </c>
       <c r="H11" s="85">
-        <v>0.19179389312977099</v>
+        <v>0.23568702290076335</v>
       </c>
       <c r="I11" s="94">
         <v>0.03</v>
       </c>
       <c r="J11" s="95">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K11" s="78">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="L11" s="79">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M11" s="94">
         <v>60</v>
@@ -1977,40 +1977,40 @@
         <v>21</v>
       </c>
       <c r="B12" s="30">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="C12" s="31">
-        <v>2212</v>
+        <v>2309</v>
       </c>
       <c r="D12" s="32">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="E12" s="32">
-        <v>1025</v>
+        <v>927</v>
       </c>
       <c r="F12" s="33">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="G12" s="84">
-        <v>0.3723916532905297</v>
+        <v>0.33547351524879615</v>
       </c>
       <c r="H12" s="85">
-        <v>0.3166512202656781</v>
+        <v>0.28646477132262049</v>
       </c>
       <c r="I12" s="94">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J12" s="95">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="K12" s="78">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="L12" s="79">
-        <v>0.56999999999999995</v>
+        <v>0.52</v>
       </c>
       <c r="M12" s="94">
-        <v>60</v>
+        <v>59.99</v>
       </c>
       <c r="N12" s="95">
         <v>59.98</v>
@@ -2019,7 +2019,7 @@
         <v>64.97</v>
       </c>
       <c r="P12" s="79">
-        <v>64.81</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="Q12" s="42">
         <v>0</v>
@@ -2033,49 +2033,49 @@
         <v>22</v>
       </c>
       <c r="B13" s="45">
-        <v>633</v>
+        <v>652</v>
       </c>
       <c r="C13" s="46">
-        <v>2326</v>
+        <v>2420</v>
       </c>
       <c r="D13" s="47">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="E13" s="47">
-        <v>1077</v>
+        <v>984</v>
       </c>
       <c r="F13" s="48">
-        <v>4385</v>
+        <v>4386</v>
       </c>
       <c r="G13" s="86">
-        <v>0.35539714867617106</v>
+        <v>0.33604887983706722</v>
       </c>
       <c r="H13" s="87">
-        <v>0.31648545401116662</v>
+        <v>0.28907168037602821</v>
       </c>
       <c r="I13" s="96">
         <v>0.11</v>
       </c>
       <c r="J13" s="97">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="K13" s="80">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="L13" s="81">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M13" s="96">
         <v>59.99</v>
       </c>
       <c r="N13" s="97">
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
       <c r="O13" s="80">
         <v>64.959999999999994</v>
       </c>
       <c r="P13" s="81">
-        <v>64.78</v>
+        <v>64.83</v>
       </c>
       <c r="Q13" s="53">
         <v>0</v>
@@ -2089,37 +2089,37 @@
         <v>23</v>
       </c>
       <c r="B14" s="45">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="C14" s="46">
-        <v>2144</v>
+        <v>2242</v>
       </c>
       <c r="D14" s="47">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E14" s="47">
-        <v>996</v>
+        <v>898</v>
       </c>
       <c r="F14" s="48">
         <v>4156</v>
       </c>
       <c r="G14" s="86">
-        <v>0.34547244094488189</v>
+        <v>0.33562992125984253</v>
       </c>
       <c r="H14" s="87">
-        <v>0.31719745222929935</v>
+        <v>0.28598726114649681</v>
       </c>
       <c r="I14" s="96">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="J14" s="97">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="K14" s="80">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="L14" s="81">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="M14" s="96">
         <v>59.99</v>
@@ -2131,7 +2131,7 @@
         <v>64.959999999999994</v>
       </c>
       <c r="P14" s="81">
-        <v>64.819999999999993</v>
+        <v>64.86</v>
       </c>
       <c r="Q14" s="53">
         <v>0</v>
@@ -2145,37 +2145,37 @@
         <v>24</v>
       </c>
       <c r="B15" s="45">
-        <v>699</v>
+        <v>718</v>
       </c>
       <c r="C15" s="46">
-        <v>1501</v>
+        <v>1582</v>
       </c>
       <c r="D15" s="47">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="E15" s="47">
-        <v>711</v>
+        <v>629</v>
       </c>
       <c r="F15" s="48">
-        <v>3277</v>
+        <v>3276</v>
       </c>
       <c r="G15" s="86">
-        <v>0.3436619718309859</v>
+        <v>0.32582159624413143</v>
       </c>
       <c r="H15" s="87">
-        <v>0.32142857142857145</v>
+        <v>0.28448665762098596</v>
       </c>
       <c r="I15" s="96">
         <v>0.12</v>
       </c>
       <c r="J15" s="97">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="K15" s="80">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="L15" s="81">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="M15" s="96">
         <v>59.99</v>
@@ -2187,7 +2187,7 @@
         <v>64.959999999999994</v>
       </c>
       <c r="P15" s="81">
-        <v>64.91</v>
+        <v>64.92</v>
       </c>
       <c r="Q15" s="53">
         <v>0</v>
@@ -2201,25 +2201,25 @@
         <v>25</v>
       </c>
       <c r="B16" s="30">
-        <v>755</v>
+        <v>745</v>
       </c>
       <c r="C16" s="31">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D16" s="32">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="E16" s="32">
         <v>450</v>
       </c>
       <c r="F16" s="33">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="G16" s="84">
-        <v>0.2662779397473275</v>
+        <v>0.2759961127308066</v>
       </c>
       <c r="H16" s="85">
-        <v>0.26071842410196988</v>
+        <v>0.2608695652173913</v>
       </c>
       <c r="I16" s="94">
         <v>0.13</v>
@@ -2228,7 +2228,7 @@
         <v>0.22</v>
       </c>
       <c r="K16" s="78">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="L16" s="79">
         <v>0.25</v>
@@ -2257,25 +2257,25 @@
         <v>26</v>
       </c>
       <c r="B17" s="30">
-        <v>824</v>
+        <v>813</v>
       </c>
       <c r="C17" s="31">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="D17" s="32">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="E17" s="32">
-        <v>423</v>
+        <v>439</v>
       </c>
       <c r="F17" s="33">
-        <v>2654</v>
+        <v>2655</v>
       </c>
       <c r="G17" s="84">
-        <v>0.26625111308993765</v>
+        <v>0.27604630454140694</v>
       </c>
       <c r="H17" s="85">
-        <v>0.27629000653167862</v>
+        <v>0.28655352480417756</v>
       </c>
       <c r="I17" s="94">
         <v>0.14000000000000001</v>
@@ -2287,7 +2287,7 @@
         <v>0.17</v>
       </c>
       <c r="L17" s="79">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="M17" s="94">
         <v>59.99</v>
@@ -2296,7 +2296,7 @@
         <v>59.99</v>
       </c>
       <c r="O17" s="78">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P17" s="79">
         <v>64.95</v>
@@ -2313,25 +2313,25 @@
         <v>27</v>
       </c>
       <c r="B18" s="30">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C18" s="31">
-        <v>1013</v>
+        <v>999</v>
       </c>
       <c r="D18" s="32">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E18" s="32">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="F18" s="33">
         <v>2697</v>
       </c>
       <c r="G18" s="84">
-        <v>0.26599845797995375</v>
+        <v>0.26754047802621433</v>
       </c>
       <c r="H18" s="85">
-        <v>0.27642857142857141</v>
+        <v>0.28642857142857142</v>
       </c>
       <c r="I18" s="94">
         <v>0.16</v>
@@ -2343,7 +2343,7 @@
         <v>0.19</v>
       </c>
       <c r="L18" s="79">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="M18" s="94">
         <v>59.99</v>
@@ -2369,25 +2369,25 @@
         <v>28</v>
       </c>
       <c r="B19" s="30">
-        <v>1110</v>
+        <v>1098</v>
       </c>
       <c r="C19" s="31">
-        <v>936</v>
+        <v>923</v>
       </c>
       <c r="D19" s="32">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="E19" s="32">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="F19" s="33">
         <v>2756</v>
       </c>
       <c r="G19" s="84">
-        <v>0.24128503075871496</v>
+        <v>0.24897400820793433</v>
       </c>
       <c r="H19" s="85">
-        <v>0.27610208816705334</v>
+        <v>0.28670788253477592</v>
       </c>
       <c r="I19" s="94">
         <v>0.19</v>
@@ -2399,7 +2399,7 @@
         <v>0.2</v>
       </c>
       <c r="L19" s="79">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="M19" s="94">
         <v>59.99</v>
@@ -2425,34 +2425,34 @@
         <v>29</v>
       </c>
       <c r="B20" s="30">
-        <v>1357</v>
+        <v>1340</v>
       </c>
       <c r="C20" s="31">
-        <v>968</v>
+        <v>954</v>
       </c>
       <c r="D20" s="32">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="E20" s="32">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="F20" s="33">
-        <v>3122</v>
+        <v>3121</v>
       </c>
       <c r="G20" s="84">
-        <v>0.23977591036414567</v>
+        <v>0.24887892376681614</v>
       </c>
       <c r="H20" s="85">
-        <v>0.27599102468212416</v>
+        <v>0.28646222887060585</v>
       </c>
       <c r="I20" s="94">
         <v>0.23</v>
       </c>
       <c r="J20" s="95">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="K20" s="78">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="L20" s="79">
         <v>0.21</v>
@@ -2481,37 +2481,37 @@
         <v>30</v>
       </c>
       <c r="B21" s="30">
-        <v>1808</v>
+        <v>1897</v>
       </c>
       <c r="C21" s="31">
-        <v>895</v>
+        <v>928</v>
       </c>
       <c r="D21" s="32">
-        <v>795</v>
+        <v>707</v>
       </c>
       <c r="E21" s="32">
-        <v>483</v>
+        <v>450</v>
       </c>
       <c r="F21" s="33">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="G21" s="84">
-        <v>0.30541682673837878</v>
+        <v>0.271505376344086</v>
       </c>
       <c r="H21" s="85">
-        <v>0.35050798258345428</v>
+        <v>0.32656023222060959</v>
       </c>
       <c r="I21" s="94">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="J21" s="95">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="K21" s="78">
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
       <c r="L21" s="79">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="M21" s="94">
         <v>59.98</v>
@@ -2520,7 +2520,7 @@
         <v>59.99</v>
       </c>
       <c r="O21" s="78">
-        <v>64.89</v>
+        <v>64.91</v>
       </c>
       <c r="P21" s="79">
         <v>64.95</v>
@@ -2537,37 +2537,37 @@
         <v>31</v>
       </c>
       <c r="B22" s="45">
-        <v>2364</v>
+        <v>2477</v>
       </c>
       <c r="C22" s="46">
-        <v>896</v>
+        <v>929</v>
       </c>
       <c r="D22" s="47">
-        <v>1014</v>
+        <v>902</v>
       </c>
       <c r="E22" s="47">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F22" s="48">
         <v>4758</v>
       </c>
       <c r="G22" s="86">
-        <v>0.30017761989342806</v>
+        <v>0.26694288250961823</v>
       </c>
       <c r="H22" s="87">
-        <v>0.35072463768115941</v>
+        <v>0.32632342277012327</v>
       </c>
       <c r="I22" s="96">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="J22" s="97">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="K22" s="80">
-        <v>0.56000000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="L22" s="81">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="M22" s="96">
         <v>59.97</v>
@@ -2576,7 +2576,7 @@
         <v>59.99</v>
       </c>
       <c r="O22" s="80">
-        <v>64.819999999999993</v>
+        <v>64.86</v>
       </c>
       <c r="P22" s="81">
         <v>64.95</v>
@@ -2593,37 +2593,37 @@
         <v>32</v>
       </c>
       <c r="B23" s="45">
-        <v>2346</v>
+        <v>2456</v>
       </c>
       <c r="C23" s="46">
-        <v>940</v>
+        <v>991</v>
       </c>
       <c r="D23" s="47">
-        <v>1005</v>
+        <v>896</v>
       </c>
       <c r="E23" s="47">
-        <v>501</v>
+        <v>450</v>
       </c>
       <c r="F23" s="48">
-        <v>4792</v>
+        <v>4793</v>
       </c>
       <c r="G23" s="86">
-        <v>0.29991047448522828</v>
+        <v>0.26730310262529833</v>
       </c>
       <c r="H23" s="87">
-        <v>0.34767522553782093</v>
+        <v>0.31228313671061764</v>
       </c>
       <c r="I23" s="96">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="J23" s="97">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="K23" s="80">
-        <v>0.56000000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="L23" s="81">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="M23" s="96">
         <v>59.97</v>
@@ -2632,10 +2632,10 @@
         <v>59.99</v>
       </c>
       <c r="O23" s="80">
-        <v>64.819999999999993</v>
+        <v>64.86</v>
       </c>
       <c r="P23" s="81">
-        <v>64.94</v>
+        <v>64.95</v>
       </c>
       <c r="Q23" s="53">
         <v>0.23</v>
@@ -2649,37 +2649,37 @@
         <v>33</v>
       </c>
       <c r="B24" s="45">
-        <v>1809</v>
+        <v>1897</v>
       </c>
       <c r="C24" s="46">
-        <v>763</v>
+        <v>790</v>
       </c>
       <c r="D24" s="47">
-        <v>795</v>
+        <v>708</v>
       </c>
       <c r="E24" s="47">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="F24" s="48">
-        <v>3817</v>
+        <v>3819</v>
       </c>
       <c r="G24" s="86">
-        <v>0.3052995391705069</v>
+        <v>0.27178502879078698</v>
       </c>
       <c r="H24" s="87">
-        <v>0.37098103874690846</v>
+        <v>0.34925864909390447</v>
       </c>
       <c r="I24" s="96">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="J24" s="97">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K24" s="80">
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
       <c r="L24" s="81">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="M24" s="96">
         <v>59.98</v>
@@ -2688,7 +2688,7 @@
         <v>59.99</v>
       </c>
       <c r="O24" s="80">
-        <v>64.89</v>
+        <v>64.91</v>
       </c>
       <c r="P24" s="81">
         <v>64.95</v>
@@ -2705,37 +2705,37 @@
         <v>34</v>
       </c>
       <c r="B25" s="30">
-        <v>1320</v>
+        <v>1303</v>
       </c>
       <c r="C25" s="31">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="D25" s="32">
-        <v>417</v>
+        <v>433</v>
       </c>
       <c r="E25" s="32">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F25" s="33">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="G25" s="84">
-        <v>0.24006908462867013</v>
+        <v>0.24942396313364054</v>
       </c>
       <c r="H25" s="85">
-        <v>0.27620221948212081</v>
+        <v>0.28641975308641976</v>
       </c>
       <c r="I25" s="94">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="J25" s="95">
         <v>0.1</v>
       </c>
       <c r="K25" s="78">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="L25" s="79">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="M25" s="94">
         <v>59.99</v>
@@ -2761,25 +2761,25 @@
         <v>35</v>
       </c>
       <c r="B26" s="30">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="C26" s="31">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D26" s="32">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="E26" s="32">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F26" s="33">
         <v>1781</v>
       </c>
       <c r="G26" s="84">
-        <v>0.26581265012009608</v>
+        <v>0.27542033626901519</v>
       </c>
       <c r="H26" s="85">
-        <v>0.27631578947368424</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I26" s="94">
         <v>0.16</v>
@@ -2788,7 +2788,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K26" s="78">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="L26" s="79">
         <v>0.08</v>
@@ -2817,37 +2817,37 @@
         <v>36</v>
       </c>
       <c r="B27" s="30">
-        <v>830</v>
+        <v>787</v>
       </c>
       <c r="C27" s="31">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="D27" s="32">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E27" s="32">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F27" s="33">
         <v>1435</v>
       </c>
       <c r="G27" s="84">
-        <v>0.18467583497053044</v>
+        <v>0.2269155206286837</v>
       </c>
       <c r="H27" s="85">
-        <v>0.19184652278177458</v>
+        <v>0.23501199040767387</v>
       </c>
       <c r="I27" s="94">
         <v>0.14000000000000001</v>
       </c>
       <c r="J27" s="95">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K27" s="78">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="L27" s="79">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="M27" s="94">
         <v>59.99</v>
@@ -2856,7 +2856,7 @@
         <v>60</v>
       </c>
       <c r="O27" s="78">
-        <v>64.98</v>
+        <v>64.97</v>
       </c>
       <c r="P27" s="79">
         <v>64.98</v>
@@ -2873,37 +2873,37 @@
         <v>37</v>
       </c>
       <c r="B28" s="30">
-        <v>691</v>
+        <v>641</v>
       </c>
       <c r="C28" s="31">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="D28" s="32">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="E28" s="32">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F28" s="33">
         <v>1022</v>
       </c>
       <c r="G28" s="84">
-        <v>6.3685636856368563E-2</v>
+        <v>0.13261163734776726</v>
       </c>
       <c r="H28" s="85">
-        <v>6.6901408450704219E-2</v>
+        <v>0.13780918727915195</v>
       </c>
       <c r="I28" s="94">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="J28" s="95">
+        <v>0.04</v>
+      </c>
+      <c r="K28" s="78">
         <v>0.05</v>
       </c>
-      <c r="K28" s="78">
-        <v>0.03</v>
-      </c>
       <c r="L28" s="79">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M28" s="94">
         <v>59.99</v>
@@ -2912,7 +2912,7 @@
         <v>60</v>
       </c>
       <c r="O28" s="78">
-        <v>64.989999999999995</v>
+        <v>64.98</v>
       </c>
       <c r="P28" s="79">
         <v>64.989999999999995</v>
@@ -2929,34 +2929,34 @@
         <v>38</v>
       </c>
       <c r="B29" s="55">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="C29" s="56">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D29" s="57">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E29" s="57">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F29" s="58">
         <v>689</v>
       </c>
       <c r="G29" s="88">
-        <v>6.3909774436090222E-2</v>
+        <v>0.13182674199623351</v>
       </c>
       <c r="H29" s="89">
-        <v>6.3694267515923567E-2</v>
+        <v>0.13924050632911392</v>
       </c>
       <c r="I29" s="98">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="J29" s="99">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="K29" s="82">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="L29" s="83">
         <v>0.01</v>
@@ -2968,7 +2968,7 @@
         <v>60</v>
       </c>
       <c r="O29" s="82">
-        <v>64.989999999999995</v>
+        <v>64.98</v>
       </c>
       <c r="P29" s="83">
         <v>64.989999999999995</v>
@@ -2986,31 +2986,31 @@
       </c>
       <c r="B30" s="65">
         <f>SUM(B6:B29)</f>
-        <v>20804</v>
+        <v>21007</v>
       </c>
       <c r="C30" s="66">
         <f t="shared" ref="C30:F30" si="0">SUM(C6:C29)</f>
-        <v>20078</v>
+        <v>20386</v>
       </c>
       <c r="D30" s="67">
         <f t="shared" si="0"/>
-        <v>7711</v>
+        <v>7509</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" si="0"/>
-        <v>8432</v>
+        <v>8124</v>
       </c>
       <c r="F30" s="68">
         <f t="shared" si="0"/>
-        <v>57025</v>
+        <v>57026</v>
       </c>
       <c r="G30" s="100">
         <f>D30/B30</f>
-        <v>0.37064987502403385</v>
+        <v>0.35745227781215783</v>
       </c>
       <c r="H30" s="101">
         <f>E30/C30</f>
-        <v>0.41996214762426537</v>
+        <v>0.39850878053566174</v>
       </c>
       <c r="I30" s="71"/>
       <c r="J30" s="71"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="B32" s="72">
         <f>B30+C30</f>
-        <v>40882</v>
+        <v>41393</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="B33" s="72">
         <f>D30+E30</f>
-        <v>16143</v>
+        <v>15633</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B34" s="72">
         <f>B32+B33</f>
-        <v>57025</v>
+        <v>57026</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3342,37 +3342,37 @@
         <v>15</v>
       </c>
       <c r="B51" s="30">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="C51" s="31">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D51" s="32">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E51" s="32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F51" s="33">
         <v>401</v>
       </c>
       <c r="G51" s="84">
-        <v>6.7961165048543687E-2</v>
+        <v>0.14239482200647249</v>
       </c>
       <c r="H51" s="85">
-        <v>5.434782608695652E-2</v>
+        <v>0.10869565217391304</v>
       </c>
       <c r="I51" s="90">
         <v>0.05</v>
       </c>
       <c r="J51" s="91">
+        <v>0.01</v>
+      </c>
+      <c r="K51" s="92">
         <v>0.02</v>
       </c>
-      <c r="K51" s="92">
+      <c r="L51" s="93">
         <v>0.01</v>
-      </c>
-      <c r="L51" s="93">
-        <v>0</v>
       </c>
       <c r="M51" s="94">
         <v>60</v>
@@ -3398,25 +3398,25 @@
         <v>16</v>
       </c>
       <c r="B52" s="30">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C52" s="31">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D52" s="32">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E52" s="32">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F52" s="33">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G52" s="84">
-        <v>6.9767441860465115E-2</v>
+        <v>0.14035087719298245</v>
       </c>
       <c r="H52" s="85">
-        <v>5.9701492537313432E-2</v>
+        <v>0.1044776119402985</v>
       </c>
       <c r="I52" s="94">
         <v>0.03</v>
@@ -3454,25 +3454,25 @@
         <v>17</v>
       </c>
       <c r="B53" s="30">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C53" s="31">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D53" s="32">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E53" s="32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F53" s="33">
         <v>177</v>
       </c>
       <c r="G53" s="84">
-        <v>6.8965517241379309E-2</v>
+        <v>0.1391304347826087</v>
       </c>
       <c r="H53" s="85">
-        <v>4.9180327868852458E-2</v>
+        <v>0.11290322580645161</v>
       </c>
       <c r="I53" s="94">
         <v>0.02</v>
@@ -3481,7 +3481,7 @@
         <v>0.01</v>
       </c>
       <c r="K53" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L53" s="79">
         <v>0</v>
@@ -3510,25 +3510,25 @@
         <v>18</v>
       </c>
       <c r="B54" s="30">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C54" s="31">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D54" s="32">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E54" s="32">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F54" s="33">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G54" s="84">
-        <v>6.5420560747663545E-2</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="H54" s="85">
-        <v>5.5555555555555552E-2</v>
+        <v>0.112</v>
       </c>
       <c r="I54" s="94">
         <v>0.02</v>
@@ -3537,10 +3537,10 @@
         <v>0.02</v>
       </c>
       <c r="K54" s="78">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L54" s="79">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M54" s="94">
         <v>60</v>
@@ -3566,37 +3566,37 @@
         <v>19</v>
       </c>
       <c r="B55" s="30">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C55" s="31">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="D55" s="32">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E55" s="32">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F55" s="33">
         <v>495</v>
       </c>
       <c r="G55" s="84">
-        <v>6.8027210884353748E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="H55" s="85">
-        <v>5.459770114942529E-2</v>
+        <v>0.11206896551724138</v>
       </c>
       <c r="I55" s="94">
         <v>0.02</v>
       </c>
       <c r="J55" s="95">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K55" s="78">
         <v>0.01</v>
       </c>
       <c r="L55" s="79">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M55" s="94">
         <v>60</v>
@@ -3622,25 +3622,25 @@
         <v>20</v>
       </c>
       <c r="B56" s="30">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C56" s="31">
-        <v>1076</v>
+        <v>1030</v>
       </c>
       <c r="D56" s="32">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E56" s="32">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="F56" s="33">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="G56" s="84">
-        <v>0.19642857142857142</v>
+        <v>0.24285714285714285</v>
       </c>
       <c r="H56" s="85">
-        <v>0.15607843137254901</v>
+        <v>0.19152276295133439</v>
       </c>
       <c r="I56" s="94">
         <v>0.04</v>
@@ -3649,10 +3649,10 @@
         <v>0.18</v>
       </c>
       <c r="K56" s="78">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="L56" s="79">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M56" s="94">
         <v>60</v>
@@ -3678,37 +3678,37 @@
         <v>21</v>
       </c>
       <c r="B57" s="30">
-        <v>461</v>
+        <v>491</v>
       </c>
       <c r="C57" s="31">
-        <v>2912</v>
+        <v>3017</v>
       </c>
       <c r="D57" s="32">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="E57" s="32">
-        <v>1028</v>
+        <v>923</v>
       </c>
       <c r="F57" s="33">
         <v>4704</v>
       </c>
       <c r="G57" s="84">
-        <v>0.39659685863874344</v>
+        <v>0.35732984293193715</v>
       </c>
       <c r="H57" s="85">
-        <v>0.26091370558375637</v>
+        <v>0.23426395939086295</v>
       </c>
       <c r="I57" s="94">
         <v>0.08</v>
       </c>
       <c r="J57" s="95">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="K57" s="78">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="L57" s="79">
-        <v>0.56999999999999995</v>
+        <v>0.51</v>
       </c>
       <c r="M57" s="94">
         <v>59.99</v>
@@ -3720,7 +3720,7 @@
         <v>64.97</v>
       </c>
       <c r="P57" s="79">
-        <v>64.81</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="Q57" s="42">
         <v>0</v>
@@ -3734,37 +3734,37 @@
         <v>22</v>
       </c>
       <c r="B58" s="45">
-        <v>754</v>
+        <v>774</v>
       </c>
       <c r="C58" s="46">
-        <v>3061</v>
+        <v>3160</v>
       </c>
       <c r="D58" s="47">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="E58" s="47">
-        <v>1082</v>
+        <v>983</v>
       </c>
       <c r="F58" s="48">
         <v>5347</v>
       </c>
       <c r="G58" s="86">
-        <v>0.37375415282392027</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="H58" s="87">
-        <v>0.26116340815833938</v>
+        <v>0.23726768042481294</v>
       </c>
       <c r="I58" s="96">
         <v>0.13</v>
       </c>
       <c r="J58" s="97">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
       <c r="K58" s="80">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="L58" s="81">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M58" s="96">
         <v>59.99</v>
@@ -3776,7 +3776,7 @@
         <v>64.95</v>
       </c>
       <c r="P58" s="81">
-        <v>64.78</v>
+        <v>64.83</v>
       </c>
       <c r="Q58" s="53">
         <v>0</v>
@@ -3790,49 +3790,49 @@
         <v>23</v>
       </c>
       <c r="B59" s="45">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="C59" s="46">
-        <v>2824</v>
+        <v>2930</v>
       </c>
       <c r="D59" s="47">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E59" s="47">
-        <v>999</v>
+        <v>894</v>
       </c>
       <c r="F59" s="48">
-        <v>5069</v>
+        <v>5071</v>
       </c>
       <c r="G59" s="86">
-        <v>0.3611556982343499</v>
+        <v>0.35685645549318362</v>
       </c>
       <c r="H59" s="87">
-        <v>0.26131310489144649</v>
+        <v>0.23378661087866109</v>
       </c>
       <c r="I59" s="96">
         <v>0.14000000000000001</v>
       </c>
       <c r="J59" s="97">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="K59" s="80">
         <v>0.25</v>
       </c>
       <c r="L59" s="81">
-        <v>0.56000000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="M59" s="96">
         <v>59.99</v>
       </c>
       <c r="N59" s="97">
-        <v>59.97</v>
+        <v>59.96</v>
       </c>
       <c r="O59" s="80">
         <v>64.95</v>
       </c>
       <c r="P59" s="81">
-        <v>64.819999999999993</v>
+        <v>64.86</v>
       </c>
       <c r="Q59" s="53">
         <v>0</v>
@@ -3846,37 +3846,37 @@
         <v>24</v>
       </c>
       <c r="B60" s="45">
-        <v>838</v>
+        <v>857</v>
       </c>
       <c r="C60" s="46">
-        <v>1987</v>
+        <v>2068</v>
       </c>
       <c r="D60" s="47">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="E60" s="47">
-        <v>705</v>
+        <v>624</v>
       </c>
       <c r="F60" s="48">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="G60" s="86">
-        <v>0.35834609494640124</v>
+        <v>0.34429992348890587</v>
       </c>
       <c r="H60" s="87">
-        <v>0.26188707280832096</v>
+        <v>0.23179791976225855</v>
       </c>
       <c r="I60" s="96">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J60" s="97">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="K60" s="80">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="L60" s="81">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="M60" s="96">
         <v>59.99</v>
@@ -3888,7 +3888,7 @@
         <v>64.95</v>
       </c>
       <c r="P60" s="81">
-        <v>64.91</v>
+        <v>64.92</v>
       </c>
       <c r="Q60" s="53">
         <v>0</v>
@@ -3902,34 +3902,34 @@
         <v>25</v>
       </c>
       <c r="B61" s="30">
-        <v>905</v>
+        <v>892</v>
       </c>
       <c r="C61" s="31">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D61" s="32">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="E61" s="32">
         <v>450</v>
       </c>
       <c r="F61" s="33">
-        <v>3364</v>
+        <v>3363</v>
       </c>
       <c r="G61" s="84">
-        <v>0.28345209817893902</v>
+        <v>0.29374505146476643</v>
       </c>
       <c r="H61" s="85">
-        <v>0.21418372203712518</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="I61" s="94">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="J61" s="95">
         <v>0.28000000000000003</v>
       </c>
       <c r="K61" s="78">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="L61" s="79">
         <v>0.25</v>
@@ -3958,25 +3958,25 @@
         <v>26</v>
       </c>
       <c r="B62" s="30">
-        <v>987</v>
+        <v>972</v>
       </c>
       <c r="C62" s="31">
-        <v>1445</v>
+        <v>1429</v>
       </c>
       <c r="D62" s="32">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="E62" s="32">
-        <v>419</v>
+        <v>435</v>
       </c>
       <c r="F62" s="33">
-        <v>3241</v>
+        <v>3240</v>
       </c>
       <c r="G62" s="84">
-        <v>0.28322440087145967</v>
+        <v>0.29360465116279072</v>
       </c>
       <c r="H62" s="85">
-        <v>0.22478540772532188</v>
+        <v>0.23336909871244635</v>
       </c>
       <c r="I62" s="94">
         <v>0.17</v>
@@ -3988,7 +3988,7 @@
         <v>0.22</v>
       </c>
       <c r="L62" s="79">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="M62" s="94">
         <v>59.99</v>
@@ -3997,7 +3997,7 @@
         <v>59.99</v>
       </c>
       <c r="O62" s="78">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="P62" s="79">
         <v>64.95</v>
@@ -4017,13 +4017,13 @@
         <v>1141</v>
       </c>
       <c r="C63" s="31">
-        <v>1321</v>
+        <v>1306</v>
       </c>
       <c r="D63" s="32">
         <v>450</v>
       </c>
       <c r="E63" s="32">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="F63" s="33">
         <v>3295</v>
@@ -4032,19 +4032,19 @@
         <v>0.28284098051539913</v>
       </c>
       <c r="H63" s="85">
-        <v>0.22476525821596244</v>
+        <v>0.2335680751173709</v>
       </c>
       <c r="I63" s="94">
         <v>0.2</v>
       </c>
       <c r="J63" s="95">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="K63" s="78">
         <v>0.25</v>
       </c>
       <c r="L63" s="79">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="M63" s="94">
         <v>59.99</v>
@@ -4070,25 +4070,25 @@
         <v>28</v>
       </c>
       <c r="B64" s="30">
-        <v>1344</v>
+        <v>1329</v>
       </c>
       <c r="C64" s="31">
-        <v>1221</v>
+        <v>1207</v>
       </c>
       <c r="D64" s="32">
-        <v>450</v>
+        <v>465</v>
       </c>
       <c r="E64" s="32">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="F64" s="33">
-        <v>3369</v>
+        <v>3368</v>
       </c>
       <c r="G64" s="84">
-        <v>0.25083612040133779</v>
+        <v>0.25919732441471571</v>
       </c>
       <c r="H64" s="85">
-        <v>0.22476190476190477</v>
+        <v>0.23316391359593391</v>
       </c>
       <c r="I64" s="94">
         <v>0.23</v>
@@ -4097,7 +4097,7 @@
         <v>0.21</v>
       </c>
       <c r="K64" s="78">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="L64" s="79">
         <v>0.2</v>
@@ -4126,37 +4126,37 @@
         <v>29</v>
       </c>
       <c r="B65" s="30">
-        <v>1643</v>
+        <v>1622</v>
       </c>
       <c r="C65" s="31">
-        <v>1261</v>
+        <v>1248</v>
       </c>
       <c r="D65" s="32">
-        <v>546</v>
+        <v>567</v>
       </c>
       <c r="E65" s="32">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="F65" s="33">
-        <v>3816</v>
+        <v>3817</v>
       </c>
       <c r="G65" s="84">
-        <v>0.2494289629968022</v>
+        <v>0.25902238465052535</v>
       </c>
       <c r="H65" s="85">
-        <v>0.22495390288875231</v>
+        <v>0.2334152334152334</v>
       </c>
       <c r="I65" s="94">
         <v>0.28000000000000003</v>
       </c>
       <c r="J65" s="95">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="K65" s="78">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="L65" s="79">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="M65" s="94">
         <v>59.98</v>
@@ -4165,7 +4165,7 @@
         <v>59.99</v>
       </c>
       <c r="O65" s="78">
-        <v>64.94</v>
+        <v>64.930000000000007</v>
       </c>
       <c r="P65" s="79">
         <v>64.959999999999994</v>
@@ -4182,37 +4182,37 @@
         <v>30</v>
       </c>
       <c r="B66" s="30">
-        <v>2143</v>
+        <v>2250</v>
       </c>
       <c r="C66" s="31">
-        <v>1198</v>
+        <v>1228</v>
       </c>
       <c r="D66" s="32">
-        <v>1050</v>
+        <v>943</v>
       </c>
       <c r="E66" s="32">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="F66" s="33">
         <v>4871</v>
       </c>
       <c r="G66" s="84">
-        <v>0.32884434700908238</v>
+        <v>0.29533354212339491</v>
       </c>
       <c r="H66" s="85">
-        <v>0.28605482717520858</v>
+        <v>0.26817640047675806</v>
       </c>
       <c r="I66" s="94">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="J66" s="95">
         <v>0.21</v>
       </c>
       <c r="K66" s="78">
-        <v>0.57999999999999996</v>
+        <v>0.52</v>
       </c>
       <c r="L66" s="79">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="M66" s="94">
         <v>59.98</v>
@@ -4221,7 +4221,7 @@
         <v>59.99</v>
       </c>
       <c r="O66" s="78">
-        <v>64.8</v>
+        <v>64.84</v>
       </c>
       <c r="P66" s="79">
         <v>64.95</v>
@@ -4238,37 +4238,37 @@
         <v>31</v>
       </c>
       <c r="B67" s="45">
-        <v>2890</v>
+        <v>2952</v>
       </c>
       <c r="C67" s="46">
-        <v>1199</v>
+        <v>1229</v>
       </c>
       <c r="D67" s="47">
-        <v>1254</v>
+        <v>1192</v>
       </c>
       <c r="E67" s="47">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="F67" s="48">
         <v>5823</v>
       </c>
       <c r="G67" s="86">
-        <v>0.30260617760617758</v>
+        <v>0.28764478764478763</v>
       </c>
       <c r="H67" s="87">
-        <v>0.28588445503275761</v>
+        <v>0.26801667659321027</v>
       </c>
       <c r="I67" s="96">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="J67" s="97">
         <v>0.21</v>
       </c>
       <c r="K67" s="80">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="L67" s="81">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="M67" s="96">
         <v>59.96</v>
@@ -4277,13 +4277,13 @@
         <v>59.99</v>
       </c>
       <c r="O67" s="80">
-        <v>64.64</v>
+        <v>64.7</v>
       </c>
       <c r="P67" s="81">
         <v>64.95</v>
       </c>
       <c r="Q67" s="53">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="R67" s="54">
         <v>0</v>
@@ -4294,37 +4294,37 @@
         <v>32</v>
       </c>
       <c r="B68" s="45">
-        <v>2858</v>
+        <v>2927</v>
       </c>
       <c r="C68" s="46">
-        <v>1257</v>
+        <v>1305</v>
       </c>
       <c r="D68" s="47">
-        <v>1253</v>
+        <v>1184</v>
       </c>
       <c r="E68" s="47">
-        <v>497</v>
+        <v>450</v>
       </c>
       <c r="F68" s="48">
-        <v>5865</v>
+        <v>5866</v>
       </c>
       <c r="G68" s="86">
-        <v>0.30479202140598394</v>
+        <v>0.28800778399416199</v>
       </c>
       <c r="H68" s="87">
-        <v>0.28335233751425315</v>
+        <v>0.25641025641025639</v>
       </c>
       <c r="I68" s="96">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="J68" s="97">
         <v>0.22</v>
       </c>
       <c r="K68" s="80">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="L68" s="81">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="M68" s="96">
         <v>59.96</v>
@@ -4333,13 +4333,13 @@
         <v>59.99</v>
       </c>
       <c r="O68" s="80">
-        <v>64.64</v>
+        <v>64.709999999999994</v>
       </c>
       <c r="P68" s="81">
-        <v>64.94</v>
+        <v>64.95</v>
       </c>
       <c r="Q68" s="53">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="R68" s="54">
         <v>0</v>
@@ -4350,37 +4350,37 @@
         <v>33</v>
       </c>
       <c r="B69" s="45">
-        <v>2145</v>
+        <v>2250</v>
       </c>
       <c r="C69" s="46">
-        <v>1027</v>
+        <v>1057</v>
       </c>
       <c r="D69" s="47">
-        <v>1050</v>
+        <v>945</v>
       </c>
       <c r="E69" s="47">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="F69" s="48">
         <v>4672</v>
       </c>
       <c r="G69" s="86">
-        <v>0.32863849765258218</v>
+        <v>0.29577464788732394</v>
       </c>
       <c r="H69" s="87">
-        <v>0.30467163168584971</v>
+        <v>0.28436018957345971</v>
       </c>
       <c r="I69" s="96">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="J69" s="97">
         <v>0.18</v>
       </c>
       <c r="K69" s="80">
-        <v>0.57999999999999996</v>
+        <v>0.52</v>
       </c>
       <c r="L69" s="81">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="M69" s="96">
         <v>59.98</v>
@@ -4389,7 +4389,7 @@
         <v>59.99</v>
       </c>
       <c r="O69" s="80">
-        <v>64.8</v>
+        <v>64.84</v>
       </c>
       <c r="P69" s="81">
         <v>64.95</v>
@@ -4406,25 +4406,25 @@
         <v>34</v>
       </c>
       <c r="B70" s="30">
-        <v>1598</v>
+        <v>1577</v>
       </c>
       <c r="C70" s="31">
-        <v>765</v>
+        <v>756</v>
       </c>
       <c r="D70" s="32">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="E70" s="32">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="F70" s="33">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="G70" s="84">
-        <v>0.24976525821596243</v>
+        <v>0.25927665570690467</v>
       </c>
       <c r="H70" s="85">
-        <v>0.22492401215805471</v>
+        <v>0.23326572008113591</v>
       </c>
       <c r="I70" s="94">
         <v>0.27</v>
@@ -4433,10 +4433,10 @@
         <v>0.13</v>
       </c>
       <c r="K70" s="78">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="L70" s="79">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="M70" s="94">
         <v>59.99</v>
@@ -4451,7 +4451,7 @@
         <v>64.97</v>
       </c>
       <c r="Q70" s="42">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="R70" s="43">
         <v>0</v>
@@ -4462,25 +4462,25 @@
         <v>35</v>
       </c>
       <c r="B71" s="30">
-        <v>1099</v>
+        <v>1083</v>
       </c>
       <c r="C71" s="31">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D71" s="32">
-        <v>434</v>
+        <v>449</v>
       </c>
       <c r="E71" s="32">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F71" s="33">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="G71" s="84">
-        <v>0.28310502283105021</v>
+        <v>0.29308093994778067</v>
       </c>
       <c r="H71" s="85">
-        <v>0.22530864197530864</v>
+        <v>0.2330246913580247</v>
       </c>
       <c r="I71" s="94">
         <v>0.19</v>
@@ -4489,7 +4489,7 @@
         <v>0.09</v>
       </c>
       <c r="K71" s="78">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="L71" s="79">
         <v>0.08</v>
@@ -4518,37 +4518,37 @@
         <v>36</v>
       </c>
       <c r="B72" s="30">
-        <v>1003</v>
+        <v>947</v>
       </c>
       <c r="C72" s="31">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="D72" s="32">
-        <v>246</v>
+        <v>302</v>
       </c>
       <c r="E72" s="32">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F72" s="33">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="G72" s="84">
-        <v>0.19695756605284229</v>
+        <v>0.24179343474779824</v>
       </c>
       <c r="H72" s="85">
-        <v>0.15551181102362205</v>
+        <v>0.19132149901380671</v>
       </c>
       <c r="I72" s="94">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J72" s="95">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K72" s="78">
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="L72" s="79">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="M72" s="94">
         <v>59.99</v>
@@ -4574,37 +4574,37 @@
         <v>37</v>
       </c>
       <c r="B73" s="30">
-        <v>844</v>
+        <v>778</v>
       </c>
       <c r="C73" s="31">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D73" s="32">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="E73" s="32">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F73" s="33">
         <v>1250</v>
       </c>
       <c r="G73" s="84">
-        <v>6.8432671081677707E-2</v>
+        <v>0.141280353200883</v>
       </c>
       <c r="H73" s="85">
-        <v>5.232558139534884E-2</v>
+        <v>0.11046511627906977</v>
       </c>
       <c r="I73" s="94">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="J73" s="95">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K73" s="78">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L73" s="79">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M73" s="94">
         <v>59.99</v>
@@ -4613,7 +4613,7 @@
         <v>60</v>
       </c>
       <c r="O73" s="78">
-        <v>64.989999999999995</v>
+        <v>64.98</v>
       </c>
       <c r="P73" s="79">
         <v>64.989999999999995</v>
@@ -4630,25 +4630,25 @@
         <v>38</v>
       </c>
       <c r="B74" s="55">
-        <v>607</v>
+        <v>560</v>
       </c>
       <c r="C74" s="56">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D74" s="57">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="E74" s="57">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F74" s="58">
         <v>843</v>
       </c>
       <c r="G74" s="88">
-        <v>6.9018404907975464E-2</v>
+        <v>0.1411042944785276</v>
       </c>
       <c r="H74" s="89">
-        <v>5.2356020942408377E-2</v>
+        <v>0.1099476439790576</v>
       </c>
       <c r="I74" s="98">
         <v>0.1</v>
@@ -4657,7 +4657,7 @@
         <v>0.03</v>
       </c>
       <c r="K74" s="82">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="L74" s="83">
         <v>0.01</v>
@@ -4669,7 +4669,7 @@
         <v>60</v>
       </c>
       <c r="O74" s="82">
-        <v>64.989999999999995</v>
+        <v>64.98</v>
       </c>
       <c r="P74" s="83">
         <v>64.989999999999995</v>
@@ -4687,31 +4687,31 @@
       </c>
       <c r="B75" s="65">
         <f>SUM(B51:B74)</f>
-        <v>25074</v>
+        <v>25145</v>
       </c>
       <c r="C75" s="66">
         <f t="shared" ref="C75" si="1">SUM(C51:C74)</f>
-        <v>26299</v>
+        <v>26620</v>
       </c>
       <c r="D75" s="67">
         <f t="shared" ref="D75" si="2">SUM(D51:D74)</f>
-        <v>9904</v>
+        <v>9830</v>
       </c>
       <c r="E75" s="67">
         <f t="shared" ref="E75" si="3">SUM(E51:E74)</f>
-        <v>8405</v>
+        <v>8082</v>
       </c>
       <c r="F75" s="68">
         <f t="shared" ref="F75" si="4">SUM(F51:F74)</f>
-        <v>69682</v>
+        <v>69677</v>
       </c>
       <c r="G75" s="100">
         <f>D75/B75</f>
-        <v>0.3949908271516312</v>
+        <v>0.39093259097236033</v>
       </c>
       <c r="H75" s="101">
         <f>E75/C75</f>
-        <v>0.31959390090877982</v>
+        <v>0.30360631104432756</v>
       </c>
       <c r="I75" s="71"/>
       <c r="J75" s="71"/>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="B77" s="72">
         <f>B75+C75</f>
-        <v>51373</v>
+        <v>51765</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B78" s="72">
         <f>D75+E75</f>
-        <v>18309</v>
+        <v>17912</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="B79" s="72">
         <f>B77+B78</f>
-        <v>69682</v>
+        <v>69677</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -15236,16 +15236,64 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="M48:P48"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="G723:H723"/>
+    <mergeCell ref="I723:L723"/>
+    <mergeCell ref="M723:P723"/>
+    <mergeCell ref="Q723:R723"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="G633:H633"/>
+    <mergeCell ref="I633:L633"/>
+    <mergeCell ref="M633:P633"/>
+    <mergeCell ref="Q633:R633"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="G678:H678"/>
+    <mergeCell ref="I678:L678"/>
+    <mergeCell ref="M678:P678"/>
+    <mergeCell ref="Q678:R678"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="G543:H543"/>
+    <mergeCell ref="I543:L543"/>
+    <mergeCell ref="M543:P543"/>
+    <mergeCell ref="Q543:R543"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="G588:H588"/>
+    <mergeCell ref="I588:L588"/>
+    <mergeCell ref="M588:P588"/>
+    <mergeCell ref="Q588:R588"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="G453:H453"/>
+    <mergeCell ref="I453:L453"/>
+    <mergeCell ref="M453:P453"/>
+    <mergeCell ref="Q453:R453"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="G498:H498"/>
+    <mergeCell ref="I498:L498"/>
+    <mergeCell ref="M498:P498"/>
+    <mergeCell ref="Q498:R498"/>
+    <mergeCell ref="Q408:R408"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="G363:H363"/>
+    <mergeCell ref="I363:L363"/>
+    <mergeCell ref="M363:P363"/>
+    <mergeCell ref="Q363:R363"/>
+    <mergeCell ref="G228:H228"/>
+    <mergeCell ref="I228:L228"/>
+    <mergeCell ref="M228:P228"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="G408:H408"/>
+    <mergeCell ref="I408:L408"/>
+    <mergeCell ref="M408:P408"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="G273:H273"/>
+    <mergeCell ref="I273:L273"/>
+    <mergeCell ref="M273:P273"/>
+    <mergeCell ref="Q273:R273"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="G318:H318"/>
+    <mergeCell ref="I318:L318"/>
+    <mergeCell ref="M318:P318"/>
+    <mergeCell ref="Q318:R318"/>
     <mergeCell ref="Q228:R228"/>
     <mergeCell ref="B93:F93"/>
     <mergeCell ref="G93:H93"/>
@@ -15262,64 +15310,16 @@
     <mergeCell ref="I183:L183"/>
     <mergeCell ref="M183:P183"/>
     <mergeCell ref="Q183:R183"/>
-    <mergeCell ref="Q273:R273"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="G318:H318"/>
-    <mergeCell ref="I318:L318"/>
-    <mergeCell ref="M318:P318"/>
-    <mergeCell ref="Q318:R318"/>
-    <mergeCell ref="G228:H228"/>
-    <mergeCell ref="I228:L228"/>
-    <mergeCell ref="M228:P228"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="G408:H408"/>
-    <mergeCell ref="I408:L408"/>
-    <mergeCell ref="M408:P408"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="G273:H273"/>
-    <mergeCell ref="I273:L273"/>
-    <mergeCell ref="M273:P273"/>
-    <mergeCell ref="Q408:R408"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="G363:H363"/>
-    <mergeCell ref="I363:L363"/>
-    <mergeCell ref="M363:P363"/>
-    <mergeCell ref="Q363:R363"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="G498:H498"/>
-    <mergeCell ref="I498:L498"/>
-    <mergeCell ref="M498:P498"/>
-    <mergeCell ref="Q498:R498"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="G453:H453"/>
-    <mergeCell ref="I453:L453"/>
-    <mergeCell ref="M453:P453"/>
-    <mergeCell ref="Q453:R453"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="G588:H588"/>
-    <mergeCell ref="I588:L588"/>
-    <mergeCell ref="M588:P588"/>
-    <mergeCell ref="Q588:R588"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="G543:H543"/>
-    <mergeCell ref="I543:L543"/>
-    <mergeCell ref="M543:P543"/>
-    <mergeCell ref="Q543:R543"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="G678:H678"/>
-    <mergeCell ref="I678:L678"/>
-    <mergeCell ref="M678:P678"/>
-    <mergeCell ref="Q678:R678"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="G633:H633"/>
-    <mergeCell ref="I633:L633"/>
-    <mergeCell ref="M633:P633"/>
-    <mergeCell ref="Q633:R633"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="G723:H723"/>
-    <mergeCell ref="I723:L723"/>
-    <mergeCell ref="M723:P723"/>
-    <mergeCell ref="Q723:R723"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="M48:P48"/>
+    <mergeCell ref="Q48:R48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scale constants the relativeness across time periods (consistent scaling)
Peak period is first adjusted and then using proportions to original peak period to other peroids, th eoothr period constanst are scaled
</commit_message>
<xml_diff>
--- a/Analysis & Profiles/Output_2020A2.xlsx
+++ b/Analysis & Profiles/Output_2020A2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\Veterans ELToDv2.3 2017-0628\Analysis &amp; Profiles\Veterans 2017-0801_newpp_revisedparams_aawdt_for_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\Veterans ELToDv2.3 2017-0628\Analysis &amp; Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1183,6 +1183,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>116542</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>545279</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47371</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8973671" y="1613647"/>
+          <a:ext cx="8066667" cy="2028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1448,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,25 +1690,25 @@
         <v>15</v>
       </c>
       <c r="B6" s="30">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="C6" s="31">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D6" s="32">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E6" s="32">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="33">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G6" s="84">
-        <v>0.13147410358565736</v>
+        <v>7.1713147410358571E-2</v>
       </c>
       <c r="H6" s="85">
-        <v>0.13333333333333333</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="I6" s="90">
         <v>0.04</v>
@@ -1668,10 +1717,10 @@
         <v>0.01</v>
       </c>
       <c r="K6" s="92">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="L6" s="93">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M6" s="94">
         <v>60</v>
@@ -1697,25 +1746,25 @@
         <v>16</v>
       </c>
       <c r="B7" s="30">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C7" s="31">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D7" s="32">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E7" s="32">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F7" s="33">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G7" s="84">
-        <v>0.1357142857142857</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="H7" s="85">
-        <v>0.14285714285714285</v>
+        <v>7.2727272727272724E-2</v>
       </c>
       <c r="I7" s="94">
         <v>0.02</v>
@@ -1753,34 +1802,34 @@
         <v>17</v>
       </c>
       <c r="B8" s="30">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C8" s="31">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D8" s="32">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8" s="32">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8" s="33">
         <v>145</v>
       </c>
       <c r="G8" s="84">
-        <v>0.1276595744680851</v>
+        <v>7.4468085106382975E-2</v>
       </c>
       <c r="H8" s="85">
-        <v>0.13725490196078433</v>
+        <v>7.8431372549019607E-2</v>
       </c>
       <c r="I8" s="94">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="J8" s="95">
         <v>0.01</v>
       </c>
       <c r="K8" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L8" s="79">
         <v>0</v>
@@ -1809,25 +1858,25 @@
         <v>18</v>
       </c>
       <c r="B9" s="30">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C9" s="31">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D9" s="32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9" s="32">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F9" s="33">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G9" s="84">
-        <v>0.13636363636363635</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="H9" s="85">
-        <v>0.13592233009708737</v>
+        <v>7.7669902912621352E-2</v>
       </c>
       <c r="I9" s="94">
         <v>0.01</v>
@@ -1836,10 +1885,10 @@
         <v>0.02</v>
       </c>
       <c r="K9" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L9" s="79">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M9" s="94">
         <v>60</v>
@@ -1865,37 +1914,37 @@
         <v>19</v>
       </c>
       <c r="B10" s="30">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C10" s="31">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="D10" s="32">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E10" s="32">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F10" s="33">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G10" s="84">
-        <v>0.13333333333333333</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H10" s="85">
-        <v>0.13636363636363635</v>
+        <v>7.3684210526315783E-2</v>
       </c>
       <c r="I10" s="94">
         <v>0.02</v>
       </c>
       <c r="J10" s="95">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="K10" s="78">
+        <v>0</v>
+      </c>
+      <c r="L10" s="79">
         <v>0.01</v>
-      </c>
-      <c r="L10" s="79">
-        <v>0.02</v>
       </c>
       <c r="M10" s="94">
         <v>60</v>
@@ -1921,37 +1970,37 @@
         <v>20</v>
       </c>
       <c r="B11" s="30">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="C11" s="31">
-        <v>801</v>
+        <v>883</v>
       </c>
       <c r="D11" s="32">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E11" s="32">
-        <v>247</v>
+        <v>165</v>
       </c>
       <c r="F11" s="33">
         <v>1277</v>
       </c>
       <c r="G11" s="84">
-        <v>0.22707423580786026</v>
+        <v>0.15283842794759825</v>
       </c>
       <c r="H11" s="85">
-        <v>0.23568702290076335</v>
+        <v>0.15744274809160305</v>
       </c>
       <c r="I11" s="94">
         <v>0.03</v>
       </c>
       <c r="J11" s="95">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="K11" s="78">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="L11" s="79">
-        <v>0.14000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="M11" s="94">
         <v>60</v>
@@ -1963,7 +2012,7 @@
         <v>64.989999999999995</v>
       </c>
       <c r="P11" s="79">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="Q11" s="42">
         <v>0</v>
@@ -1977,49 +2026,49 @@
         <v>21</v>
       </c>
       <c r="B12" s="30">
-        <v>414</v>
+        <v>450</v>
       </c>
       <c r="C12" s="31">
-        <v>2309</v>
+        <v>2477</v>
       </c>
       <c r="D12" s="32">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="E12" s="32">
-        <v>927</v>
+        <v>759</v>
       </c>
       <c r="F12" s="33">
         <v>3859</v>
       </c>
       <c r="G12" s="84">
-        <v>0.33547351524879615</v>
+        <v>0.27768860353130015</v>
       </c>
       <c r="H12" s="85">
-        <v>0.28646477132262049</v>
+        <v>0.23454882571075403</v>
       </c>
       <c r="I12" s="94">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="J12" s="95">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="K12" s="78">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="L12" s="79">
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
       <c r="M12" s="94">
         <v>59.99</v>
       </c>
       <c r="N12" s="95">
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
       <c r="O12" s="78">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="P12" s="79">
-        <v>64.849999999999994</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="Q12" s="42">
         <v>0</v>
@@ -2033,37 +2082,37 @@
         <v>22</v>
       </c>
       <c r="B13" s="45">
-        <v>652</v>
+        <v>710</v>
       </c>
       <c r="C13" s="46">
-        <v>2420</v>
+        <v>2584</v>
       </c>
       <c r="D13" s="47">
-        <v>330</v>
+        <v>272</v>
       </c>
       <c r="E13" s="47">
-        <v>984</v>
+        <v>819</v>
       </c>
       <c r="F13" s="48">
-        <v>4386</v>
+        <v>4385</v>
       </c>
       <c r="G13" s="86">
-        <v>0.33604887983706722</v>
+        <v>0.27698574338085541</v>
       </c>
       <c r="H13" s="87">
-        <v>0.28907168037602821</v>
+        <v>0.2406699970614164</v>
       </c>
       <c r="I13" s="96">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="J13" s="97">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="K13" s="80">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="L13" s="81">
-        <v>0.55000000000000004</v>
+        <v>0.46</v>
       </c>
       <c r="M13" s="96">
         <v>59.99</v>
@@ -2072,10 +2121,10 @@
         <v>59.97</v>
       </c>
       <c r="O13" s="80">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P13" s="81">
-        <v>64.83</v>
+        <v>64.88</v>
       </c>
       <c r="Q13" s="53">
         <v>0</v>
@@ -2089,49 +2138,49 @@
         <v>23</v>
       </c>
       <c r="B14" s="45">
-        <v>675</v>
+        <v>735</v>
       </c>
       <c r="C14" s="46">
-        <v>2242</v>
+        <v>2409</v>
       </c>
       <c r="D14" s="47">
-        <v>341</v>
+        <v>281</v>
       </c>
       <c r="E14" s="47">
-        <v>898</v>
+        <v>732</v>
       </c>
       <c r="F14" s="48">
-        <v>4156</v>
+        <v>4157</v>
       </c>
       <c r="G14" s="86">
-        <v>0.33562992125984253</v>
+        <v>0.27657480314960631</v>
       </c>
       <c r="H14" s="87">
-        <v>0.28598726114649681</v>
+        <v>0.23304680038204392</v>
       </c>
       <c r="I14" s="96">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="J14" s="97">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="K14" s="80">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="L14" s="81">
-        <v>0.5</v>
+        <v>0.41</v>
       </c>
       <c r="M14" s="96">
         <v>59.99</v>
       </c>
       <c r="N14" s="97">
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
       <c r="O14" s="80">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P14" s="81">
-        <v>64.86</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="Q14" s="53">
         <v>0</v>
@@ -2145,55 +2194,55 @@
         <v>24</v>
       </c>
       <c r="B15" s="45">
-        <v>718</v>
+        <v>770</v>
       </c>
       <c r="C15" s="46">
-        <v>1582</v>
+        <v>1686</v>
       </c>
       <c r="D15" s="47">
-        <v>347</v>
+        <v>295</v>
       </c>
       <c r="E15" s="47">
-        <v>629</v>
+        <v>526</v>
       </c>
       <c r="F15" s="48">
-        <v>3276</v>
+        <v>3277</v>
       </c>
       <c r="G15" s="86">
-        <v>0.32582159624413143</v>
+        <v>0.27699530516431925</v>
       </c>
       <c r="H15" s="87">
-        <v>0.28448665762098596</v>
+        <v>0.23779385171790235</v>
       </c>
       <c r="I15" s="96">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="J15" s="97">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K15" s="80">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="L15" s="81">
-        <v>0.35</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="M15" s="96">
         <v>59.99</v>
       </c>
       <c r="N15" s="97">
-        <v>59.99</v>
+        <v>59.98</v>
       </c>
       <c r="O15" s="80">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P15" s="81">
-        <v>64.92</v>
+        <v>64.94</v>
       </c>
       <c r="Q15" s="53">
         <v>0</v>
       </c>
       <c r="R15" s="54">
-        <v>0.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2201,37 +2250,37 @@
         <v>25</v>
       </c>
       <c r="B16" s="30">
-        <v>745</v>
+        <v>818</v>
       </c>
       <c r="C16" s="31">
-        <v>1275</v>
+        <v>1359</v>
       </c>
       <c r="D16" s="32">
-        <v>284</v>
+        <v>211</v>
       </c>
       <c r="E16" s="32">
-        <v>450</v>
+        <v>366</v>
       </c>
       <c r="F16" s="33">
         <v>2754</v>
       </c>
       <c r="G16" s="84">
-        <v>0.2759961127308066</v>
+        <v>0.20505344995140914</v>
       </c>
       <c r="H16" s="85">
-        <v>0.2608695652173913</v>
+        <v>0.21217391304347827</v>
       </c>
       <c r="I16" s="94">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J16" s="95">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="K16" s="78">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="L16" s="79">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="M16" s="94">
         <v>59.99</v>
@@ -2243,7 +2292,7 @@
         <v>64.97</v>
       </c>
       <c r="P16" s="79">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q16" s="42">
         <v>0</v>
@@ -2257,37 +2306,37 @@
         <v>26</v>
       </c>
       <c r="B17" s="30">
-        <v>813</v>
+        <v>892</v>
       </c>
       <c r="C17" s="31">
-        <v>1093</v>
+        <v>1206</v>
       </c>
       <c r="D17" s="32">
-        <v>310</v>
+        <v>230</v>
       </c>
       <c r="E17" s="32">
-        <v>439</v>
+        <v>325</v>
       </c>
       <c r="F17" s="33">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="G17" s="84">
-        <v>0.27604630454140694</v>
+        <v>0.20499108734402852</v>
       </c>
       <c r="H17" s="85">
-        <v>0.28655352480417756</v>
+        <v>0.2122795558458524</v>
       </c>
       <c r="I17" s="94">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J17" s="95">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="K17" s="78">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="L17" s="79">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="M17" s="94">
         <v>59.99</v>
@@ -2296,10 +2345,10 @@
         <v>59.99</v>
       </c>
       <c r="O17" s="78">
+        <v>64.97</v>
+      </c>
+      <c r="P17" s="79">
         <v>64.959999999999994</v>
-      </c>
-      <c r="P17" s="79">
-        <v>64.95</v>
       </c>
       <c r="Q17" s="42">
         <v>0</v>
@@ -2313,37 +2362,37 @@
         <v>27</v>
       </c>
       <c r="B18" s="30">
-        <v>950</v>
+        <v>1031</v>
       </c>
       <c r="C18" s="31">
-        <v>999</v>
+        <v>1103</v>
       </c>
       <c r="D18" s="32">
-        <v>347</v>
+        <v>266</v>
       </c>
       <c r="E18" s="32">
-        <v>401</v>
+        <v>297</v>
       </c>
       <c r="F18" s="33">
         <v>2697</v>
       </c>
       <c r="G18" s="84">
-        <v>0.26754047802621433</v>
+        <v>0.20508866615265997</v>
       </c>
       <c r="H18" s="85">
-        <v>0.28642857142857142</v>
+        <v>0.21214285714285713</v>
       </c>
       <c r="I18" s="94">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="J18" s="95">
+        <v>0.19</v>
+      </c>
+      <c r="K18" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="L18" s="79">
         <v>0.17</v>
-      </c>
-      <c r="K18" s="78">
-        <v>0.19</v>
-      </c>
-      <c r="L18" s="79">
-        <v>0.22</v>
       </c>
       <c r="M18" s="94">
         <v>59.99</v>
@@ -2352,10 +2401,10 @@
         <v>59.99</v>
       </c>
       <c r="O18" s="78">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P18" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q18" s="42">
         <v>0</v>
@@ -2369,37 +2418,37 @@
         <v>28</v>
       </c>
       <c r="B19" s="30">
-        <v>1098</v>
+        <v>1163</v>
       </c>
       <c r="C19" s="31">
-        <v>923</v>
+        <v>1019</v>
       </c>
       <c r="D19" s="32">
-        <v>364</v>
+        <v>300</v>
       </c>
       <c r="E19" s="32">
-        <v>371</v>
+        <v>275</v>
       </c>
       <c r="F19" s="33">
-        <v>2756</v>
+        <v>2757</v>
       </c>
       <c r="G19" s="84">
-        <v>0.24897400820793433</v>
+        <v>0.20505809979494191</v>
       </c>
       <c r="H19" s="85">
-        <v>0.28670788253477592</v>
+        <v>0.21251931993817619</v>
       </c>
       <c r="I19" s="94">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="J19" s="95">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="K19" s="78">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="L19" s="79">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="M19" s="94">
         <v>59.99</v>
@@ -2408,10 +2457,10 @@
         <v>59.99</v>
       </c>
       <c r="O19" s="78">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P19" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q19" s="42">
         <v>0</v>
@@ -2425,37 +2474,37 @@
         <v>29</v>
       </c>
       <c r="B20" s="30">
-        <v>1340</v>
+        <v>1436</v>
       </c>
       <c r="C20" s="31">
-        <v>954</v>
+        <v>1053</v>
       </c>
       <c r="D20" s="32">
-        <v>444</v>
+        <v>348</v>
       </c>
       <c r="E20" s="32">
-        <v>383</v>
+        <v>284</v>
       </c>
       <c r="F20" s="33">
         <v>3121</v>
       </c>
       <c r="G20" s="84">
-        <v>0.24887892376681614</v>
+        <v>0.19506726457399104</v>
       </c>
       <c r="H20" s="85">
-        <v>0.28646222887060585</v>
+        <v>0.21241585639491398</v>
       </c>
       <c r="I20" s="94">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="J20" s="95">
+        <v>0.18</v>
+      </c>
+      <c r="K20" s="78">
+        <v>0.19</v>
+      </c>
+      <c r="L20" s="79">
         <v>0.16</v>
-      </c>
-      <c r="K20" s="78">
-        <v>0.25</v>
-      </c>
-      <c r="L20" s="79">
-        <v>0.21</v>
       </c>
       <c r="M20" s="94">
         <v>59.99</v>
@@ -2464,10 +2513,10 @@
         <v>59.99</v>
       </c>
       <c r="O20" s="78">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P20" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q20" s="42">
         <v>0</v>
@@ -2481,37 +2530,37 @@
         <v>30</v>
       </c>
       <c r="B21" s="30">
-        <v>1897</v>
+        <v>2031</v>
       </c>
       <c r="C21" s="31">
-        <v>928</v>
+        <v>982</v>
       </c>
       <c r="D21" s="32">
-        <v>707</v>
+        <v>572</v>
       </c>
       <c r="E21" s="32">
-        <v>450</v>
+        <v>396</v>
       </c>
       <c r="F21" s="33">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="G21" s="84">
-        <v>0.271505376344086</v>
+        <v>0.21974644640799079</v>
       </c>
       <c r="H21" s="85">
-        <v>0.32656023222060959</v>
+        <v>0.28737300435413643</v>
       </c>
       <c r="I21" s="94">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="J21" s="95">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="K21" s="78">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
       <c r="L21" s="79">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="M21" s="94">
         <v>59.98</v>
@@ -2520,10 +2569,10 @@
         <v>59.99</v>
       </c>
       <c r="O21" s="78">
-        <v>64.91</v>
+        <v>64.930000000000007</v>
       </c>
       <c r="P21" s="79">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q21" s="42">
         <v>0.23</v>
@@ -2537,37 +2586,37 @@
         <v>31</v>
       </c>
       <c r="B22" s="45">
-        <v>2477</v>
+        <v>2635</v>
       </c>
       <c r="C22" s="46">
-        <v>929</v>
+        <v>983</v>
       </c>
       <c r="D22" s="47">
-        <v>902</v>
+        <v>743</v>
       </c>
       <c r="E22" s="47">
-        <v>450</v>
+        <v>397</v>
       </c>
       <c r="F22" s="48">
         <v>4758</v>
       </c>
       <c r="G22" s="86">
-        <v>0.26694288250961823</v>
+        <v>0.21995263469508586</v>
       </c>
       <c r="H22" s="87">
-        <v>0.32632342277012327</v>
+        <v>0.28768115942028988</v>
       </c>
       <c r="I22" s="96">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="J22" s="97">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="K22" s="80">
-        <v>0.5</v>
+        <v>0.41</v>
       </c>
       <c r="L22" s="81">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="M22" s="96">
         <v>59.97</v>
@@ -2576,10 +2625,10 @@
         <v>59.99</v>
       </c>
       <c r="O22" s="80">
-        <v>64.86</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="P22" s="81">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q22" s="53">
         <v>0.23</v>
@@ -2593,37 +2642,37 @@
         <v>32</v>
       </c>
       <c r="B23" s="45">
-        <v>2456</v>
+        <v>2614</v>
       </c>
       <c r="C23" s="46">
-        <v>991</v>
+        <v>1027</v>
       </c>
       <c r="D23" s="47">
-        <v>896</v>
+        <v>737</v>
       </c>
       <c r="E23" s="47">
-        <v>450</v>
+        <v>414</v>
       </c>
       <c r="F23" s="48">
-        <v>4793</v>
+        <v>4792</v>
       </c>
       <c r="G23" s="86">
-        <v>0.26730310262529833</v>
+        <v>0.21993434795583408</v>
       </c>
       <c r="H23" s="87">
-        <v>0.31228313671061764</v>
+        <v>0.28730048577376821</v>
       </c>
       <c r="I23" s="96">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="J23" s="97">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="K23" s="80">
-        <v>0.5</v>
+        <v>0.41</v>
       </c>
       <c r="L23" s="81">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="M23" s="96">
         <v>59.97</v>
@@ -2632,7 +2681,7 @@
         <v>59.99</v>
       </c>
       <c r="O23" s="80">
-        <v>64.86</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="P23" s="81">
         <v>64.95</v>
@@ -2649,37 +2698,37 @@
         <v>33</v>
       </c>
       <c r="B24" s="45">
-        <v>1897</v>
+        <v>2032</v>
       </c>
       <c r="C24" s="46">
-        <v>790</v>
+        <v>865</v>
       </c>
       <c r="D24" s="47">
-        <v>708</v>
+        <v>572</v>
       </c>
       <c r="E24" s="47">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="F24" s="48">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="G24" s="86">
-        <v>0.27178502879078698</v>
+        <v>0.2196620583717358</v>
       </c>
       <c r="H24" s="87">
-        <v>0.34925864909390447</v>
+        <v>0.28747940691927515</v>
       </c>
       <c r="I24" s="96">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="J24" s="97">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="K24" s="80">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
       <c r="L24" s="81">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="M24" s="96">
         <v>59.98</v>
@@ -2688,10 +2737,10 @@
         <v>59.99</v>
       </c>
       <c r="O24" s="80">
-        <v>64.91</v>
+        <v>64.930000000000007</v>
       </c>
       <c r="P24" s="81">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q24" s="53">
         <v>0.23</v>
@@ -2705,37 +2754,37 @@
         <v>34</v>
       </c>
       <c r="B25" s="30">
-        <v>1303</v>
+        <v>1390</v>
       </c>
       <c r="C25" s="31">
-        <v>578</v>
+        <v>638</v>
       </c>
       <c r="D25" s="32">
-        <v>433</v>
+        <v>346</v>
       </c>
       <c r="E25" s="32">
-        <v>232</v>
+        <v>172</v>
       </c>
       <c r="F25" s="33">
         <v>2546</v>
       </c>
       <c r="G25" s="84">
-        <v>0.24942396313364054</v>
+        <v>0.19930875576036866</v>
       </c>
       <c r="H25" s="85">
-        <v>0.28641975308641976</v>
+        <v>0.21234567901234569</v>
       </c>
       <c r="I25" s="94">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="J25" s="95">
+        <v>0.11</v>
+      </c>
+      <c r="K25" s="78">
+        <v>0.19</v>
+      </c>
+      <c r="L25" s="79">
         <v>0.1</v>
-      </c>
-      <c r="K25" s="78">
-        <v>0.24</v>
-      </c>
-      <c r="L25" s="79">
-        <v>0.13</v>
       </c>
       <c r="M25" s="94">
         <v>59.99</v>
@@ -2744,10 +2793,10 @@
         <v>59.99</v>
       </c>
       <c r="O25" s="78">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P25" s="79">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="Q25" s="42">
         <v>0</v>
@@ -2761,46 +2810,46 @@
         <v>35</v>
       </c>
       <c r="B26" s="30">
-        <v>905</v>
+        <v>994</v>
       </c>
       <c r="C26" s="31">
-        <v>380</v>
+        <v>419</v>
       </c>
       <c r="D26" s="32">
-        <v>344</v>
+        <v>255</v>
       </c>
       <c r="E26" s="32">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="F26" s="33">
         <v>1781</v>
       </c>
       <c r="G26" s="84">
-        <v>0.27542033626901519</v>
+        <v>0.20416333066453163</v>
       </c>
       <c r="H26" s="85">
-        <v>0.2857142857142857</v>
+        <v>0.21240601503759399</v>
       </c>
       <c r="I26" s="94">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="J26" s="95">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K26" s="78">
-        <v>0.19</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L26" s="79">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="M26" s="94">
         <v>59.99</v>
       </c>
       <c r="N26" s="95">
-        <v>60</v>
+        <v>59.99</v>
       </c>
       <c r="O26" s="78">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="P26" s="79">
         <v>64.98</v>
@@ -2817,37 +2866,37 @@
         <v>36</v>
       </c>
       <c r="B27" s="30">
-        <v>787</v>
+        <v>864</v>
       </c>
       <c r="C27" s="31">
-        <v>319</v>
+        <v>351</v>
       </c>
       <c r="D27" s="32">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="E27" s="32">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F27" s="33">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="G27" s="84">
-        <v>0.2269155206286837</v>
+        <v>0.1521099116781158</v>
       </c>
       <c r="H27" s="85">
-        <v>0.23501199040767387</v>
+        <v>0.15827338129496402</v>
       </c>
       <c r="I27" s="94">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J27" s="95">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K27" s="78">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="L27" s="79">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M27" s="94">
         <v>59.99</v>
@@ -2856,10 +2905,10 @@
         <v>60</v>
       </c>
       <c r="O27" s="78">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="P27" s="79">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="Q27" s="42">
         <v>0</v>
@@ -2873,37 +2922,37 @@
         <v>37</v>
       </c>
       <c r="B28" s="30">
-        <v>641</v>
+        <v>685</v>
       </c>
       <c r="C28" s="31">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="D28" s="32">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E28" s="32">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F28" s="33">
         <v>1022</v>
       </c>
       <c r="G28" s="84">
-        <v>0.13261163734776726</v>
+        <v>7.307171853856563E-2</v>
       </c>
       <c r="H28" s="85">
-        <v>0.13780918727915195</v>
+        <v>7.4204946996466431E-2</v>
       </c>
       <c r="I28" s="94">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="J28" s="95">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="K28" s="78">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="L28" s="79">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M28" s="94">
         <v>59.99</v>
@@ -2912,7 +2961,7 @@
         <v>60</v>
       </c>
       <c r="O28" s="78">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="P28" s="79">
         <v>64.989999999999995</v>
@@ -2929,34 +2978,34 @@
         <v>38</v>
       </c>
       <c r="B29" s="55">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="C29" s="56">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D29" s="57">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E29" s="57">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F29" s="58">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="G29" s="88">
-        <v>0.13182674199623351</v>
+        <v>7.3308270676691725E-2</v>
       </c>
       <c r="H29" s="89">
-        <v>0.13924050632911392</v>
+        <v>7.5949367088607597E-2</v>
       </c>
       <c r="I29" s="98">
         <v>0.08</v>
       </c>
       <c r="J29" s="99">
+        <v>0.03</v>
+      </c>
+      <c r="K29" s="82">
         <v>0.02</v>
-      </c>
-      <c r="K29" s="82">
-        <v>0.04</v>
       </c>
       <c r="L29" s="83">
         <v>0.01</v>
@@ -2968,7 +3017,7 @@
         <v>60</v>
       </c>
       <c r="O29" s="82">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="P29" s="83">
         <v>64.989999999999995</v>
@@ -2986,31 +3035,31 @@
       </c>
       <c r="B30" s="65">
         <f>SUM(B6:B29)</f>
-        <v>21007</v>
+        <v>22579</v>
       </c>
       <c r="C30" s="66">
         <f t="shared" ref="C30:F30" si="0">SUM(C6:C29)</f>
-        <v>20386</v>
+        <v>21979</v>
       </c>
       <c r="D30" s="67">
         <f t="shared" si="0"/>
-        <v>7509</v>
+        <v>5934</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" si="0"/>
-        <v>8124</v>
+        <v>6531</v>
       </c>
       <c r="F30" s="68">
         <f t="shared" si="0"/>
-        <v>57026</v>
+        <v>57023</v>
       </c>
       <c r="G30" s="100">
         <f>D30/B30</f>
-        <v>0.35745227781215783</v>
+        <v>0.26281057619912307</v>
       </c>
       <c r="H30" s="101">
         <f>E30/C30</f>
-        <v>0.39850878053566174</v>
+        <v>0.29714727694617588</v>
       </c>
       <c r="I30" s="71"/>
       <c r="J30" s="71"/>
@@ -3023,7 +3072,7 @@
       </c>
       <c r="B32" s="72">
         <f>B30+C30</f>
-        <v>41393</v>
+        <v>44558</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -3032,7 +3081,7 @@
       </c>
       <c r="B33" s="72">
         <f>D30+E30</f>
-        <v>15633</v>
+        <v>12465</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3041,7 +3090,7 @@
       </c>
       <c r="B34" s="72">
         <f>B32+B33</f>
-        <v>57026</v>
+        <v>57023</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3342,25 +3391,25 @@
         <v>15</v>
       </c>
       <c r="B51" s="30">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="C51" s="31">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D51" s="32">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E51" s="32">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F51" s="33">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G51" s="84">
-        <v>0.14239482200647249</v>
+        <v>7.7669902912621352E-2</v>
       </c>
       <c r="H51" s="85">
-        <v>0.10869565217391304</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="I51" s="90">
         <v>0.05</v>
@@ -3369,10 +3418,10 @@
         <v>0.01</v>
       </c>
       <c r="K51" s="92">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="L51" s="93">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M51" s="94">
         <v>60</v>
@@ -3398,25 +3447,25 @@
         <v>16</v>
       </c>
       <c r="B52" s="30">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C52" s="31">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D52" s="32">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E52" s="32">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F52" s="33">
         <v>238</v>
       </c>
       <c r="G52" s="84">
-        <v>0.14035087719298245</v>
+        <v>7.6023391812865493E-2</v>
       </c>
       <c r="H52" s="85">
-        <v>0.1044776119402985</v>
+        <v>5.9701492537313432E-2</v>
       </c>
       <c r="I52" s="94">
         <v>0.03</v>
@@ -3454,25 +3503,25 @@
         <v>17</v>
       </c>
       <c r="B53" s="30">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C53" s="31">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D53" s="32">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E53" s="32">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F53" s="33">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G53" s="84">
-        <v>0.1391304347826087</v>
+        <v>7.7586206896551727E-2</v>
       </c>
       <c r="H53" s="85">
-        <v>0.11290322580645161</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="I53" s="94">
         <v>0.02</v>
@@ -3481,7 +3530,7 @@
         <v>0.01</v>
       </c>
       <c r="K53" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L53" s="79">
         <v>0</v>
@@ -3510,25 +3559,25 @@
         <v>18</v>
       </c>
       <c r="B54" s="30">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C54" s="31">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D54" s="32">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E54" s="32">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F54" s="33">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G54" s="84">
-        <v>0.14018691588785046</v>
+        <v>7.476635514018691E-2</v>
       </c>
       <c r="H54" s="85">
-        <v>0.112</v>
+        <v>6.3492063492063489E-2</v>
       </c>
       <c r="I54" s="94">
         <v>0.02</v>
@@ -3537,10 +3586,10 @@
         <v>0.02</v>
       </c>
       <c r="K54" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L54" s="79">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M54" s="94">
         <v>60</v>
@@ -3566,37 +3615,37 @@
         <v>19</v>
       </c>
       <c r="B55" s="30">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C55" s="31">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="D55" s="32">
+        <v>11</v>
+      </c>
+      <c r="E55" s="32">
         <v>21</v>
-      </c>
-      <c r="E55" s="32">
-        <v>39</v>
       </c>
       <c r="F55" s="33">
         <v>495</v>
       </c>
       <c r="G55" s="84">
-        <v>0.14285714285714285</v>
+        <v>7.4829931972789115E-2</v>
       </c>
       <c r="H55" s="85">
-        <v>0.11206896551724138</v>
+        <v>6.0344827586206899E-2</v>
       </c>
       <c r="I55" s="94">
         <v>0.02</v>
       </c>
       <c r="J55" s="95">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K55" s="78">
         <v>0.01</v>
       </c>
       <c r="L55" s="79">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M55" s="94">
         <v>60</v>
@@ -3622,37 +3671,37 @@
         <v>20</v>
       </c>
       <c r="B56" s="30">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="C56" s="31">
-        <v>1030</v>
+        <v>1112</v>
       </c>
       <c r="D56" s="32">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="E56" s="32">
-        <v>244</v>
+        <v>163</v>
       </c>
       <c r="F56" s="33">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="G56" s="84">
-        <v>0.24285714285714285</v>
+        <v>0.16071428571428573</v>
       </c>
       <c r="H56" s="85">
-        <v>0.19152276295133439</v>
+        <v>0.12784313725490196</v>
       </c>
       <c r="I56" s="94">
         <v>0.04</v>
       </c>
       <c r="J56" s="95">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="K56" s="78">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="L56" s="79">
-        <v>0.14000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="M56" s="94">
         <v>60</v>
@@ -3664,7 +3713,7 @@
         <v>64.989999999999995</v>
       </c>
       <c r="P56" s="79">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="Q56" s="42">
         <v>0</v>
@@ -3678,49 +3727,49 @@
         <v>21</v>
       </c>
       <c r="B57" s="30">
-        <v>491</v>
+        <v>539</v>
       </c>
       <c r="C57" s="31">
-        <v>3017</v>
+        <v>3182</v>
       </c>
       <c r="D57" s="32">
-        <v>273</v>
+        <v>225</v>
       </c>
       <c r="E57" s="32">
-        <v>923</v>
+        <v>758</v>
       </c>
       <c r="F57" s="33">
         <v>4704</v>
       </c>
       <c r="G57" s="84">
-        <v>0.35732984293193715</v>
+        <v>0.29450261780104714</v>
       </c>
       <c r="H57" s="85">
-        <v>0.23426395939086295</v>
+        <v>0.19238578680203045</v>
       </c>
       <c r="I57" s="94">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="J57" s="95">
-        <v>0.52</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K57" s="78">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="L57" s="79">
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="M57" s="94">
         <v>59.99</v>
       </c>
       <c r="N57" s="95">
-        <v>59.96</v>
+        <v>59.95</v>
       </c>
       <c r="O57" s="78">
         <v>64.97</v>
       </c>
       <c r="P57" s="79">
-        <v>64.849999999999994</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="Q57" s="42">
         <v>0</v>
@@ -3734,49 +3783,49 @@
         <v>22</v>
       </c>
       <c r="B58" s="45">
-        <v>774</v>
+        <v>849</v>
       </c>
       <c r="C58" s="46">
-        <v>3160</v>
+        <v>3319</v>
       </c>
       <c r="D58" s="47">
-        <v>430</v>
+        <v>355</v>
       </c>
       <c r="E58" s="47">
-        <v>983</v>
+        <v>824</v>
       </c>
       <c r="F58" s="48">
         <v>5347</v>
       </c>
       <c r="G58" s="86">
-        <v>0.35714285714285715</v>
+        <v>0.29485049833887045</v>
       </c>
       <c r="H58" s="87">
-        <v>0.23726768042481294</v>
+        <v>0.19888969345884625</v>
       </c>
       <c r="I58" s="96">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="J58" s="97">
-        <v>0.54</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K58" s="80">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="L58" s="81">
-        <v>0.55000000000000004</v>
+        <v>0.46</v>
       </c>
       <c r="M58" s="96">
         <v>59.99</v>
       </c>
       <c r="N58" s="97">
-        <v>59.96</v>
+        <v>59.95</v>
       </c>
       <c r="O58" s="80">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P58" s="81">
-        <v>64.83</v>
+        <v>64.88</v>
       </c>
       <c r="Q58" s="53">
         <v>0</v>
@@ -3790,37 +3839,37 @@
         <v>23</v>
       </c>
       <c r="B59" s="45">
-        <v>802</v>
+        <v>879</v>
       </c>
       <c r="C59" s="46">
-        <v>2930</v>
+        <v>3095</v>
       </c>
       <c r="D59" s="47">
-        <v>445</v>
+        <v>367</v>
       </c>
       <c r="E59" s="47">
-        <v>894</v>
+        <v>729</v>
       </c>
       <c r="F59" s="48">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="G59" s="86">
-        <v>0.35685645549318362</v>
+        <v>0.2945425361155698</v>
       </c>
       <c r="H59" s="87">
-        <v>0.23378661087866109</v>
+        <v>0.19063807531380753</v>
       </c>
       <c r="I59" s="96">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J59" s="97">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="K59" s="80">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="L59" s="81">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M59" s="96">
         <v>59.99</v>
@@ -3829,10 +3878,10 @@
         <v>59.96</v>
       </c>
       <c r="O59" s="80">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P59" s="81">
-        <v>64.86</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="Q59" s="53">
         <v>0</v>
@@ -3846,37 +3895,37 @@
         <v>24</v>
       </c>
       <c r="B60" s="45">
-        <v>857</v>
+        <v>922</v>
       </c>
       <c r="C60" s="46">
-        <v>2068</v>
+        <v>2171</v>
       </c>
       <c r="D60" s="47">
-        <v>450</v>
+        <v>385</v>
       </c>
       <c r="E60" s="47">
-        <v>624</v>
+        <v>521</v>
       </c>
       <c r="F60" s="48">
         <v>3999</v>
       </c>
       <c r="G60" s="86">
-        <v>0.34429992348890587</v>
+        <v>0.29456771231828616</v>
       </c>
       <c r="H60" s="87">
-        <v>0.23179791976225855</v>
+        <v>0.19353640416047549</v>
       </c>
       <c r="I60" s="96">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="J60" s="97">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="K60" s="80">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="L60" s="81">
-        <v>0.35</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="M60" s="96">
         <v>59.99</v>
@@ -3885,16 +3934,16 @@
         <v>59.98</v>
       </c>
       <c r="O60" s="80">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P60" s="81">
-        <v>64.92</v>
+        <v>64.94</v>
       </c>
       <c r="Q60" s="53">
         <v>0</v>
       </c>
       <c r="R60" s="54">
-        <v>0.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3902,37 +3951,37 @@
         <v>25</v>
       </c>
       <c r="B61" s="30">
-        <v>892</v>
+        <v>987</v>
       </c>
       <c r="C61" s="31">
-        <v>1650</v>
+        <v>1737</v>
       </c>
       <c r="D61" s="32">
-        <v>371</v>
+        <v>276</v>
       </c>
       <c r="E61" s="32">
-        <v>450</v>
+        <v>363</v>
       </c>
       <c r="F61" s="33">
         <v>3363</v>
       </c>
       <c r="G61" s="84">
-        <v>0.29374505146476643</v>
+        <v>0.21852731591448932</v>
       </c>
       <c r="H61" s="85">
-        <v>0.21428571428571427</v>
+        <v>0.17285714285714285</v>
       </c>
       <c r="I61" s="94">
+        <v>0.17</v>
+      </c>
+      <c r="J61" s="95">
+        <v>0.3</v>
+      </c>
+      <c r="K61" s="78">
         <v>0.15</v>
       </c>
-      <c r="J61" s="95">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="K61" s="78">
-        <v>0.21</v>
-      </c>
       <c r="L61" s="79">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="M61" s="94">
         <v>59.99</v>
@@ -3941,10 +3990,10 @@
         <v>59.98</v>
       </c>
       <c r="O61" s="78">
+        <v>64.97</v>
+      </c>
+      <c r="P61" s="79">
         <v>64.959999999999994</v>
-      </c>
-      <c r="P61" s="79">
-        <v>64.95</v>
       </c>
       <c r="Q61" s="42">
         <v>0</v>
@@ -3958,37 +4007,37 @@
         <v>26</v>
       </c>
       <c r="B62" s="30">
-        <v>972</v>
+        <v>1076</v>
       </c>
       <c r="C62" s="31">
-        <v>1429</v>
+        <v>1542</v>
       </c>
       <c r="D62" s="32">
-        <v>404</v>
+        <v>301</v>
       </c>
       <c r="E62" s="32">
-        <v>435</v>
+        <v>322</v>
       </c>
       <c r="F62" s="33">
-        <v>3240</v>
+        <v>3241</v>
       </c>
       <c r="G62" s="84">
-        <v>0.29360465116279072</v>
+        <v>0.21859114015976761</v>
       </c>
       <c r="H62" s="85">
-        <v>0.23336909871244635</v>
+        <v>0.17274678111587982</v>
       </c>
       <c r="I62" s="94">
+        <v>0.18</v>
+      </c>
+      <c r="J62" s="95">
+        <v>0.26</v>
+      </c>
+      <c r="K62" s="78">
         <v>0.17</v>
       </c>
-      <c r="J62" s="95">
-        <v>0.25</v>
-      </c>
-      <c r="K62" s="78">
-        <v>0.22</v>
-      </c>
       <c r="L62" s="79">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="M62" s="94">
         <v>59.99</v>
@@ -3997,10 +4046,10 @@
         <v>59.99</v>
       </c>
       <c r="O62" s="78">
-        <v>64.95</v>
+        <v>64.97</v>
       </c>
       <c r="P62" s="79">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q62" s="42">
         <v>0</v>
@@ -4014,37 +4063,37 @@
         <v>27</v>
       </c>
       <c r="B63" s="30">
-        <v>1141</v>
+        <v>1244</v>
       </c>
       <c r="C63" s="31">
-        <v>1306</v>
+        <v>1410</v>
       </c>
       <c r="D63" s="32">
-        <v>450</v>
+        <v>347</v>
       </c>
       <c r="E63" s="32">
-        <v>398</v>
+        <v>294</v>
       </c>
       <c r="F63" s="33">
         <v>3295</v>
       </c>
       <c r="G63" s="84">
-        <v>0.28284098051539913</v>
+        <v>0.21810182275298554</v>
       </c>
       <c r="H63" s="85">
-        <v>0.2335680751173709</v>
+        <v>0.17253521126760563</v>
       </c>
       <c r="I63" s="94">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="J63" s="95">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="K63" s="78">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
       <c r="L63" s="79">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="M63" s="94">
         <v>59.99</v>
@@ -4053,10 +4102,10 @@
         <v>59.99</v>
       </c>
       <c r="O63" s="78">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P63" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q63" s="42">
         <v>0</v>
@@ -4070,37 +4119,37 @@
         <v>28</v>
       </c>
       <c r="B64" s="30">
-        <v>1329</v>
+        <v>1403</v>
       </c>
       <c r="C64" s="31">
-        <v>1207</v>
+        <v>1303</v>
       </c>
       <c r="D64" s="32">
-        <v>465</v>
+        <v>392</v>
       </c>
       <c r="E64" s="32">
-        <v>367</v>
+        <v>272</v>
       </c>
       <c r="F64" s="33">
-        <v>3368</v>
+        <v>3370</v>
       </c>
       <c r="G64" s="84">
-        <v>0.25919732441471571</v>
+        <v>0.21838440111420612</v>
       </c>
       <c r="H64" s="85">
-        <v>0.23316391359593391</v>
+        <v>0.17269841269841271</v>
       </c>
       <c r="I64" s="94">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="J64" s="95">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="K64" s="78">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="L64" s="79">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="M64" s="94">
         <v>59.99</v>
@@ -4109,10 +4158,10 @@
         <v>59.99</v>
       </c>
       <c r="O64" s="78">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P64" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q64" s="42">
         <v>0</v>
@@ -4126,37 +4175,37 @@
         <v>29</v>
       </c>
       <c r="B65" s="30">
-        <v>1622</v>
+        <v>1739</v>
       </c>
       <c r="C65" s="31">
-        <v>1248</v>
+        <v>1346</v>
       </c>
       <c r="D65" s="32">
-        <v>567</v>
+        <v>450</v>
       </c>
       <c r="E65" s="32">
-        <v>380</v>
+        <v>281</v>
       </c>
       <c r="F65" s="33">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="G65" s="84">
-        <v>0.25902238465052535</v>
+        <v>0.2055733211512106</v>
       </c>
       <c r="H65" s="85">
-        <v>0.2334152334152334</v>
+        <v>0.17271051014136449</v>
       </c>
       <c r="I65" s="94">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="J65" s="95">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="K65" s="78">
-        <v>0.31</v>
+        <v>0.25</v>
       </c>
       <c r="L65" s="79">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="M65" s="94">
         <v>59.98</v>
@@ -4165,13 +4214,13 @@
         <v>59.99</v>
       </c>
       <c r="O65" s="78">
-        <v>64.930000000000007</v>
+        <v>64.95</v>
       </c>
       <c r="P65" s="79">
-        <v>64.959999999999994</v>
+        <v>64.97</v>
       </c>
       <c r="Q65" s="42">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="R65" s="43">
         <v>0</v>
@@ -4182,49 +4231,49 @@
         <v>30</v>
       </c>
       <c r="B66" s="30">
-        <v>2250</v>
+        <v>2426</v>
       </c>
       <c r="C66" s="31">
-        <v>1228</v>
+        <v>1285</v>
       </c>
       <c r="D66" s="32">
-        <v>943</v>
+        <v>767</v>
       </c>
       <c r="E66" s="32">
-        <v>450</v>
+        <v>393</v>
       </c>
       <c r="F66" s="33">
         <v>4871</v>
       </c>
       <c r="G66" s="84">
-        <v>0.29533354212339491</v>
+        <v>0.24021296586282492</v>
       </c>
       <c r="H66" s="85">
-        <v>0.26817640047675806</v>
+        <v>0.23420738974970204</v>
       </c>
       <c r="I66" s="94">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
       <c r="J66" s="95">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="K66" s="78">
-        <v>0.52</v>
+        <v>0.43</v>
       </c>
       <c r="L66" s="79">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="M66" s="94">
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
       <c r="N66" s="95">
         <v>59.99</v>
       </c>
       <c r="O66" s="78">
-        <v>64.84</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="P66" s="79">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q66" s="42">
         <v>0.23</v>
@@ -4238,37 +4287,37 @@
         <v>31</v>
       </c>
       <c r="B67" s="45">
-        <v>2952</v>
+        <v>3147</v>
       </c>
       <c r="C67" s="46">
-        <v>1229</v>
+        <v>1286</v>
       </c>
       <c r="D67" s="47">
-        <v>1192</v>
+        <v>997</v>
       </c>
       <c r="E67" s="47">
-        <v>450</v>
+        <v>393</v>
       </c>
       <c r="F67" s="48">
         <v>5823</v>
       </c>
       <c r="G67" s="86">
-        <v>0.28764478764478763</v>
+        <v>0.24058880308880309</v>
       </c>
       <c r="H67" s="87">
-        <v>0.26801667659321027</v>
+        <v>0.23406789755807028</v>
       </c>
       <c r="I67" s="96">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="J67" s="97">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="K67" s="80">
-        <v>0.66</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L67" s="81">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="M67" s="96">
         <v>59.96</v>
@@ -4277,13 +4326,13 @@
         <v>59.99</v>
       </c>
       <c r="O67" s="80">
-        <v>64.7</v>
+        <v>64.819999999999993</v>
       </c>
       <c r="P67" s="81">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q67" s="53">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="R67" s="54">
         <v>0</v>
@@ -4294,37 +4343,37 @@
         <v>32</v>
       </c>
       <c r="B68" s="45">
-        <v>2927</v>
+        <v>3122</v>
       </c>
       <c r="C68" s="46">
-        <v>1305</v>
+        <v>1344</v>
       </c>
       <c r="D68" s="47">
-        <v>1184</v>
+        <v>989</v>
       </c>
       <c r="E68" s="47">
-        <v>450</v>
+        <v>411</v>
       </c>
       <c r="F68" s="48">
         <v>5866</v>
       </c>
       <c r="G68" s="86">
-        <v>0.28800778399416199</v>
+        <v>0.24057406956944782</v>
       </c>
       <c r="H68" s="87">
-        <v>0.25641025641025639</v>
+        <v>0.23418803418803419</v>
       </c>
       <c r="I68" s="96">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="J68" s="97">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="K68" s="80">
-        <v>0.66</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L68" s="81">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="M68" s="96">
         <v>59.96</v>
@@ -4333,13 +4382,13 @@
         <v>59.99</v>
       </c>
       <c r="O68" s="80">
-        <v>64.709999999999994</v>
+        <v>64.83</v>
       </c>
       <c r="P68" s="81">
         <v>64.95</v>
       </c>
       <c r="Q68" s="53">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="R68" s="54">
         <v>0</v>
@@ -4350,49 +4399,49 @@
         <v>33</v>
       </c>
       <c r="B69" s="45">
-        <v>2250</v>
+        <v>2427</v>
       </c>
       <c r="C69" s="46">
-        <v>1057</v>
+        <v>1131</v>
       </c>
       <c r="D69" s="47">
-        <v>945</v>
+        <v>768</v>
       </c>
       <c r="E69" s="47">
-        <v>420</v>
+        <v>346</v>
       </c>
       <c r="F69" s="48">
         <v>4672</v>
       </c>
       <c r="G69" s="86">
-        <v>0.29577464788732394</v>
+        <v>0.24037558685446009</v>
       </c>
       <c r="H69" s="87">
-        <v>0.28436018957345971</v>
+        <v>0.23425863236289776</v>
       </c>
       <c r="I69" s="96">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
       <c r="J69" s="97">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="K69" s="80">
-        <v>0.52</v>
+        <v>0.43</v>
       </c>
       <c r="L69" s="81">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="M69" s="96">
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
       <c r="N69" s="97">
         <v>59.99</v>
       </c>
       <c r="O69" s="80">
-        <v>64.84</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="P69" s="81">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q69" s="53">
         <v>0.23</v>
@@ -4406,52 +4455,52 @@
         <v>34</v>
       </c>
       <c r="B70" s="30">
-        <v>1577</v>
+        <v>1680</v>
       </c>
       <c r="C70" s="31">
-        <v>756</v>
+        <v>816</v>
       </c>
       <c r="D70" s="32">
-        <v>552</v>
+        <v>450</v>
       </c>
       <c r="E70" s="32">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="F70" s="33">
-        <v>3115</v>
+        <v>3116</v>
       </c>
       <c r="G70" s="84">
-        <v>0.25927665570690467</v>
+        <v>0.21126760563380281</v>
       </c>
       <c r="H70" s="85">
-        <v>0.23326572008113591</v>
+        <v>0.17241379310344829</v>
       </c>
       <c r="I70" s="94">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J70" s="95">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K70" s="78">
-        <v>0.31</v>
+        <v>0.25</v>
       </c>
       <c r="L70" s="79">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="M70" s="94">
-        <v>59.99</v>
+        <v>59.98</v>
       </c>
       <c r="N70" s="95">
         <v>59.99</v>
       </c>
       <c r="O70" s="78">
-        <v>64.94</v>
+        <v>64.95</v>
       </c>
       <c r="P70" s="79">
-        <v>64.97</v>
+        <v>64.98</v>
       </c>
       <c r="Q70" s="42">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="R70" s="43">
         <v>0</v>
@@ -4462,37 +4511,37 @@
         <v>35</v>
       </c>
       <c r="B71" s="30">
-        <v>1083</v>
+        <v>1198</v>
       </c>
       <c r="C71" s="31">
-        <v>497</v>
+        <v>536</v>
       </c>
       <c r="D71" s="32">
-        <v>449</v>
+        <v>334</v>
       </c>
       <c r="E71" s="32">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="F71" s="33">
         <v>2180</v>
       </c>
       <c r="G71" s="84">
-        <v>0.29308093994778067</v>
+        <v>0.21801566579634465</v>
       </c>
       <c r="H71" s="85">
-        <v>0.2330246913580247</v>
+        <v>0.1728395061728395</v>
       </c>
       <c r="I71" s="94">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="J71" s="95">
         <v>0.09</v>
       </c>
       <c r="K71" s="78">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
       <c r="L71" s="79">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="M71" s="94">
         <v>59.99</v>
@@ -4501,7 +4550,7 @@
         <v>59.99</v>
       </c>
       <c r="O71" s="78">
-        <v>64.95</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P71" s="79">
         <v>64.98</v>
@@ -4518,37 +4567,37 @@
         <v>36</v>
       </c>
       <c r="B72" s="30">
-        <v>947</v>
+        <v>1047</v>
       </c>
       <c r="C72" s="31">
-        <v>410</v>
+        <v>443</v>
       </c>
       <c r="D72" s="32">
-        <v>302</v>
+        <v>203</v>
       </c>
       <c r="E72" s="32">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="F72" s="33">
-        <v>1756</v>
+        <v>1758</v>
       </c>
       <c r="G72" s="84">
-        <v>0.24179343474779824</v>
+        <v>0.16239999999999999</v>
       </c>
       <c r="H72" s="85">
-        <v>0.19132149901380671</v>
+        <v>0.12795275590551181</v>
       </c>
       <c r="I72" s="94">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="J72" s="95">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="K72" s="78">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="L72" s="79">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M72" s="94">
         <v>59.99</v>
@@ -4560,7 +4609,7 @@
         <v>64.97</v>
       </c>
       <c r="P72" s="79">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="Q72" s="42">
         <v>0</v>
@@ -4574,37 +4623,37 @@
         <v>37</v>
       </c>
       <c r="B73" s="30">
-        <v>778</v>
+        <v>836</v>
       </c>
       <c r="C73" s="31">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="D73" s="32">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="E73" s="32">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F73" s="33">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="G73" s="84">
-        <v>0.141280353200883</v>
+        <v>7.7262693156732898E-2</v>
       </c>
       <c r="H73" s="85">
-        <v>0.11046511627906977</v>
+        <v>6.0869565217391307E-2</v>
       </c>
       <c r="I73" s="94">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J73" s="95">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K73" s="78">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="L73" s="79">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M73" s="94">
         <v>59.99</v>
@@ -4630,25 +4679,25 @@
         <v>38</v>
       </c>
       <c r="B74" s="55">
-        <v>560</v>
+        <v>601</v>
       </c>
       <c r="C74" s="56">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D74" s="57">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="E74" s="57">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F74" s="58">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="G74" s="88">
-        <v>0.1411042944785276</v>
+        <v>7.8220858895705528E-2</v>
       </c>
       <c r="H74" s="89">
-        <v>0.1099476439790576</v>
+        <v>6.25E-2</v>
       </c>
       <c r="I74" s="98">
         <v>0.1</v>
@@ -4657,7 +4706,7 @@
         <v>0.03</v>
       </c>
       <c r="K74" s="82">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="L74" s="83">
         <v>0.01</v>
@@ -4669,7 +4718,7 @@
         <v>60</v>
       </c>
       <c r="O74" s="82">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="P74" s="83">
         <v>64.989999999999995</v>
@@ -4687,31 +4736,31 @@
       </c>
       <c r="B75" s="65">
         <f>SUM(B51:B74)</f>
-        <v>25145</v>
+        <v>27142</v>
       </c>
       <c r="C75" s="66">
         <f t="shared" ref="C75" si="1">SUM(C51:C74)</f>
-        <v>26620</v>
+        <v>28215</v>
       </c>
       <c r="D75" s="67">
         <f t="shared" ref="D75" si="2">SUM(D51:D74)</f>
-        <v>9830</v>
+        <v>7837</v>
       </c>
       <c r="E75" s="67">
         <f t="shared" ref="E75" si="3">SUM(E51:E74)</f>
-        <v>8082</v>
+        <v>6493</v>
       </c>
       <c r="F75" s="68">
         <f t="shared" ref="F75" si="4">SUM(F51:F74)</f>
-        <v>69677</v>
+        <v>69687</v>
       </c>
       <c r="G75" s="100">
         <f>D75/B75</f>
-        <v>0.39093259097236033</v>
+        <v>0.28874069707464445</v>
       </c>
       <c r="H75" s="101">
         <f>E75/C75</f>
-        <v>0.30360631104432756</v>
+        <v>0.23012581959950382</v>
       </c>
       <c r="I75" s="71"/>
       <c r="J75" s="71"/>
@@ -4724,7 +4773,7 @@
       </c>
       <c r="B77" s="72">
         <f>B75+C75</f>
-        <v>51765</v>
+        <v>55357</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -4733,7 +4782,7 @@
       </c>
       <c r="B78" s="72">
         <f>D75+E75</f>
-        <v>17912</v>
+        <v>14330</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -4742,7 +4791,7 @@
       </c>
       <c r="B79" s="72">
         <f>B77+B78</f>
-        <v>69677</v>
+        <v>69687</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -15236,64 +15285,16 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="G723:H723"/>
-    <mergeCell ref="I723:L723"/>
-    <mergeCell ref="M723:P723"/>
-    <mergeCell ref="Q723:R723"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="G633:H633"/>
-    <mergeCell ref="I633:L633"/>
-    <mergeCell ref="M633:P633"/>
-    <mergeCell ref="Q633:R633"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="G678:H678"/>
-    <mergeCell ref="I678:L678"/>
-    <mergeCell ref="M678:P678"/>
-    <mergeCell ref="Q678:R678"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="G543:H543"/>
-    <mergeCell ref="I543:L543"/>
-    <mergeCell ref="M543:P543"/>
-    <mergeCell ref="Q543:R543"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="G588:H588"/>
-    <mergeCell ref="I588:L588"/>
-    <mergeCell ref="M588:P588"/>
-    <mergeCell ref="Q588:R588"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="G453:H453"/>
-    <mergeCell ref="I453:L453"/>
-    <mergeCell ref="M453:P453"/>
-    <mergeCell ref="Q453:R453"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="G498:H498"/>
-    <mergeCell ref="I498:L498"/>
-    <mergeCell ref="M498:P498"/>
-    <mergeCell ref="Q498:R498"/>
-    <mergeCell ref="Q408:R408"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="G363:H363"/>
-    <mergeCell ref="I363:L363"/>
-    <mergeCell ref="M363:P363"/>
-    <mergeCell ref="Q363:R363"/>
-    <mergeCell ref="G228:H228"/>
-    <mergeCell ref="I228:L228"/>
-    <mergeCell ref="M228:P228"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="G408:H408"/>
-    <mergeCell ref="I408:L408"/>
-    <mergeCell ref="M408:P408"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="G273:H273"/>
-    <mergeCell ref="I273:L273"/>
-    <mergeCell ref="M273:P273"/>
-    <mergeCell ref="Q273:R273"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="G318:H318"/>
-    <mergeCell ref="I318:L318"/>
-    <mergeCell ref="M318:P318"/>
-    <mergeCell ref="Q318:R318"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="M48:P48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="Q228:R228"/>
     <mergeCell ref="B93:F93"/>
     <mergeCell ref="G93:H93"/>
@@ -15310,17 +15311,66 @@
     <mergeCell ref="I183:L183"/>
     <mergeCell ref="M183:P183"/>
     <mergeCell ref="Q183:R183"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="M48:P48"/>
-    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="Q273:R273"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="G318:H318"/>
+    <mergeCell ref="I318:L318"/>
+    <mergeCell ref="M318:P318"/>
+    <mergeCell ref="Q318:R318"/>
+    <mergeCell ref="G228:H228"/>
+    <mergeCell ref="I228:L228"/>
+    <mergeCell ref="M228:P228"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="G408:H408"/>
+    <mergeCell ref="I408:L408"/>
+    <mergeCell ref="M408:P408"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="G273:H273"/>
+    <mergeCell ref="I273:L273"/>
+    <mergeCell ref="M273:P273"/>
+    <mergeCell ref="Q408:R408"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="G363:H363"/>
+    <mergeCell ref="I363:L363"/>
+    <mergeCell ref="M363:P363"/>
+    <mergeCell ref="Q363:R363"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="G498:H498"/>
+    <mergeCell ref="I498:L498"/>
+    <mergeCell ref="M498:P498"/>
+    <mergeCell ref="Q498:R498"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="G453:H453"/>
+    <mergeCell ref="I453:L453"/>
+    <mergeCell ref="M453:P453"/>
+    <mergeCell ref="Q453:R453"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="G588:H588"/>
+    <mergeCell ref="I588:L588"/>
+    <mergeCell ref="M588:P588"/>
+    <mergeCell ref="Q588:R588"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="G543:H543"/>
+    <mergeCell ref="I543:L543"/>
+    <mergeCell ref="M543:P543"/>
+    <mergeCell ref="Q543:R543"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="G678:H678"/>
+    <mergeCell ref="I678:L678"/>
+    <mergeCell ref="M678:P678"/>
+    <mergeCell ref="Q678:R678"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="G633:H633"/>
+    <mergeCell ref="I633:L633"/>
+    <mergeCell ref="M633:P633"/>
+    <mergeCell ref="Q633:R633"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="G723:H723"/>
+    <mergeCell ref="I723:L723"/>
+    <mergeCell ref="M723:P723"/>
+    <mergeCell ref="Q723:R723"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scale hourly constants with VOT_ratio_I95_xpress_reverse
</commit_message>
<xml_diff>
--- a/Analysis & Profiles/Output_2020A2.xlsx
+++ b/Analysis & Profiles/Output_2020A2.xlsx
@@ -1183,55 +1183,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>116542</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>170329</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>545279</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47371</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8973671" y="1613647"/>
-          <a:ext cx="8066667" cy="2028571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1498,7 +1449,7 @@
   <dimension ref="A1:R764"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,25 +1641,25 @@
         <v>15</v>
       </c>
       <c r="B6" s="30">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C6" s="31">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="32">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" s="33">
         <v>327</v>
       </c>
       <c r="G6" s="84">
-        <v>7.1713147410358571E-2</v>
+        <v>5.1792828685258967E-2</v>
       </c>
       <c r="H6" s="85">
-        <v>7.8947368421052627E-2</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="I6" s="90">
         <v>0.04</v>
@@ -1746,25 +1697,25 @@
         <v>16</v>
       </c>
       <c r="B7" s="30">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C7" s="31">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="32">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="33">
         <v>195</v>
       </c>
       <c r="G7" s="84">
-        <v>7.1428571428571425E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H7" s="85">
-        <v>7.2727272727272724E-2</v>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="I7" s="94">
         <v>0.02</v>
@@ -1773,7 +1724,7 @@
         <v>0.01</v>
       </c>
       <c r="K7" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L7" s="79">
         <v>0</v>
@@ -1802,25 +1753,25 @@
         <v>17</v>
       </c>
       <c r="B8" s="30">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C8" s="31">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="33">
         <v>145</v>
       </c>
       <c r="G8" s="84">
-        <v>7.4468085106382975E-2</v>
+        <v>5.3191489361702128E-2</v>
       </c>
       <c r="H8" s="85">
-        <v>7.8431372549019607E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="I8" s="94">
         <v>0.02</v>
@@ -1858,25 +1809,25 @@
         <v>18</v>
       </c>
       <c r="B9" s="30">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C9" s="31">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D9" s="32">
+        <v>5</v>
+      </c>
+      <c r="E9" s="32">
         <v>6</v>
       </c>
-      <c r="E9" s="32">
-        <v>8</v>
-      </c>
       <c r="F9" s="33">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G9" s="84">
-        <v>6.8965517241379309E-2</v>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="H9" s="85">
-        <v>7.7669902912621352E-2</v>
+        <v>5.8252427184466021E-2</v>
       </c>
       <c r="I9" s="94">
         <v>0.01</v>
@@ -1914,25 +1865,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="30">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C10" s="31">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D10" s="32">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E10" s="32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F10" s="33">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G10" s="84">
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H10" s="85">
-        <v>7.3684210526315783E-2</v>
+        <v>5.5944055944055944E-2</v>
       </c>
       <c r="I10" s="94">
         <v>0.02</v>
@@ -1970,25 +1921,25 @@
         <v>20</v>
       </c>
       <c r="B11" s="30">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C11" s="31">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="D11" s="32">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="32">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F11" s="33">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="G11" s="84">
-        <v>0.15283842794759825</v>
+        <v>0.15789473684210525</v>
       </c>
       <c r="H11" s="85">
-        <v>0.15744274809160305</v>
+        <v>0.16412213740458015</v>
       </c>
       <c r="I11" s="94">
         <v>0.03</v>
@@ -2000,7 +1951,7 @@
         <v>0.02</v>
       </c>
       <c r="L11" s="79">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="M11" s="94">
         <v>60</v>
@@ -2026,49 +1977,49 @@
         <v>21</v>
       </c>
       <c r="B12" s="30">
-        <v>450</v>
+        <v>414</v>
       </c>
       <c r="C12" s="31">
-        <v>2477</v>
+        <v>2309</v>
       </c>
       <c r="D12" s="32">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="E12" s="32">
-        <v>759</v>
+        <v>927</v>
       </c>
       <c r="F12" s="33">
         <v>3859</v>
       </c>
       <c r="G12" s="84">
-        <v>0.27768860353130015</v>
+        <v>0.33547351524879615</v>
       </c>
       <c r="H12" s="85">
-        <v>0.23454882571075403</v>
+        <v>0.28646477132262049</v>
       </c>
       <c r="I12" s="94">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J12" s="95">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="K12" s="78">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="L12" s="79">
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="M12" s="94">
         <v>59.99</v>
       </c>
       <c r="N12" s="95">
-        <v>59.97</v>
+        <v>59.98</v>
       </c>
       <c r="O12" s="78">
-        <v>64.98</v>
+        <v>64.97</v>
       </c>
       <c r="P12" s="79">
-        <v>64.900000000000006</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="Q12" s="42">
         <v>0</v>
@@ -2082,37 +2033,37 @@
         <v>22</v>
       </c>
       <c r="B13" s="45">
-        <v>710</v>
+        <v>652</v>
       </c>
       <c r="C13" s="46">
-        <v>2584</v>
+        <v>2420</v>
       </c>
       <c r="D13" s="47">
-        <v>272</v>
+        <v>330</v>
       </c>
       <c r="E13" s="47">
-        <v>819</v>
+        <v>984</v>
       </c>
       <c r="F13" s="48">
-        <v>4385</v>
+        <v>4386</v>
       </c>
       <c r="G13" s="86">
-        <v>0.27698574338085541</v>
+        <v>0.33604887983706722</v>
       </c>
       <c r="H13" s="87">
-        <v>0.2406699970614164</v>
+        <v>0.28907168037602821</v>
       </c>
       <c r="I13" s="96">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="J13" s="97">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="K13" s="80">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="L13" s="81">
-        <v>0.46</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M13" s="96">
         <v>59.99</v>
@@ -2121,10 +2072,10 @@
         <v>59.97</v>
       </c>
       <c r="O13" s="80">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P13" s="81">
-        <v>64.88</v>
+        <v>64.83</v>
       </c>
       <c r="Q13" s="53">
         <v>0</v>
@@ -2138,49 +2089,49 @@
         <v>23</v>
       </c>
       <c r="B14" s="45">
-        <v>735</v>
+        <v>675</v>
       </c>
       <c r="C14" s="46">
-        <v>2409</v>
+        <v>2242</v>
       </c>
       <c r="D14" s="47">
-        <v>281</v>
+        <v>341</v>
       </c>
       <c r="E14" s="47">
-        <v>732</v>
+        <v>898</v>
       </c>
       <c r="F14" s="48">
-        <v>4157</v>
+        <v>4156</v>
       </c>
       <c r="G14" s="86">
-        <v>0.27657480314960631</v>
+        <v>0.33562992125984253</v>
       </c>
       <c r="H14" s="87">
-        <v>0.23304680038204392</v>
+        <v>0.28598726114649681</v>
       </c>
       <c r="I14" s="96">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="J14" s="97">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="K14" s="80">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="L14" s="81">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="M14" s="96">
         <v>59.99</v>
       </c>
       <c r="N14" s="97">
-        <v>59.97</v>
+        <v>59.98</v>
       </c>
       <c r="O14" s="80">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P14" s="81">
-        <v>64.900000000000006</v>
+        <v>64.86</v>
       </c>
       <c r="Q14" s="53">
         <v>0</v>
@@ -2194,55 +2145,55 @@
         <v>24</v>
       </c>
       <c r="B15" s="45">
-        <v>770</v>
+        <v>718</v>
       </c>
       <c r="C15" s="46">
-        <v>1686</v>
+        <v>1582</v>
       </c>
       <c r="D15" s="47">
-        <v>295</v>
+        <v>347</v>
       </c>
       <c r="E15" s="47">
-        <v>526</v>
+        <v>629</v>
       </c>
       <c r="F15" s="48">
-        <v>3277</v>
+        <v>3276</v>
       </c>
       <c r="G15" s="86">
-        <v>0.27699530516431925</v>
+        <v>0.32582159624413143</v>
       </c>
       <c r="H15" s="87">
-        <v>0.23779385171790235</v>
+        <v>0.28448665762098596</v>
       </c>
       <c r="I15" s="96">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="J15" s="97">
-        <v>0.28999999999999998</v>
+        <v>0.27</v>
       </c>
       <c r="K15" s="80">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="L15" s="81">
-        <v>0.28999999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="M15" s="96">
         <v>59.99</v>
       </c>
       <c r="N15" s="97">
-        <v>59.98</v>
+        <v>59.99</v>
       </c>
       <c r="O15" s="80">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P15" s="81">
-        <v>64.94</v>
+        <v>64.92</v>
       </c>
       <c r="Q15" s="53">
         <v>0</v>
       </c>
       <c r="R15" s="54">
-        <v>0</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2250,37 +2201,37 @@
         <v>25</v>
       </c>
       <c r="B16" s="30">
-        <v>818</v>
+        <v>790</v>
       </c>
       <c r="C16" s="31">
-        <v>1359</v>
+        <v>1309</v>
       </c>
       <c r="D16" s="32">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="E16" s="32">
-        <v>366</v>
+        <v>417</v>
       </c>
       <c r="F16" s="33">
-        <v>2754</v>
+        <v>2755</v>
       </c>
       <c r="G16" s="84">
-        <v>0.20505344995140914</v>
+        <v>0.23226433430515064</v>
       </c>
       <c r="H16" s="85">
-        <v>0.21217391304347827</v>
+        <v>0.24159907300115874</v>
       </c>
       <c r="I16" s="94">
         <v>0.14000000000000001</v>
       </c>
       <c r="J16" s="95">
+        <v>0.22</v>
+      </c>
+      <c r="K16" s="78">
+        <v>0.13</v>
+      </c>
+      <c r="L16" s="79">
         <v>0.23</v>
-      </c>
-      <c r="K16" s="78">
-        <v>0.12</v>
-      </c>
-      <c r="L16" s="79">
-        <v>0.2</v>
       </c>
       <c r="M16" s="94">
         <v>59.99</v>
@@ -2292,7 +2243,7 @@
         <v>64.97</v>
       </c>
       <c r="P16" s="79">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q16" s="42">
         <v>0</v>
@@ -2306,37 +2257,37 @@
         <v>26</v>
       </c>
       <c r="B17" s="30">
-        <v>892</v>
+        <v>861</v>
       </c>
       <c r="C17" s="31">
-        <v>1206</v>
+        <v>1162</v>
       </c>
       <c r="D17" s="32">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="E17" s="32">
-        <v>325</v>
+        <v>370</v>
       </c>
       <c r="F17" s="33">
-        <v>2653</v>
+        <v>2654</v>
       </c>
       <c r="G17" s="84">
-        <v>0.20499108734402852</v>
+        <v>0.23262032085561499</v>
       </c>
       <c r="H17" s="85">
-        <v>0.2122795558458524</v>
+        <v>0.24151436031331594</v>
       </c>
       <c r="I17" s="94">
         <v>0.15</v>
       </c>
       <c r="J17" s="95">
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="L17" s="79">
         <v>0.21</v>
-      </c>
-      <c r="K17" s="78">
-        <v>0.13</v>
-      </c>
-      <c r="L17" s="79">
-        <v>0.18</v>
       </c>
       <c r="M17" s="94">
         <v>59.99</v>
@@ -2362,37 +2313,37 @@
         <v>27</v>
       </c>
       <c r="B18" s="30">
-        <v>1031</v>
+        <v>995</v>
       </c>
       <c r="C18" s="31">
-        <v>1103</v>
+        <v>1062</v>
       </c>
       <c r="D18" s="32">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="E18" s="32">
-        <v>297</v>
+        <v>338</v>
       </c>
       <c r="F18" s="33">
         <v>2697</v>
       </c>
       <c r="G18" s="84">
-        <v>0.20508866615265997</v>
+        <v>0.23284502698535081</v>
       </c>
       <c r="H18" s="85">
-        <v>0.21214285714285713</v>
+        <v>0.24142857142857144</v>
       </c>
       <c r="I18" s="94">
+        <v>0.17</v>
+      </c>
+      <c r="J18" s="95">
         <v>0.18</v>
       </c>
-      <c r="J18" s="95">
+      <c r="K18" s="78">
+        <v>0.17</v>
+      </c>
+      <c r="L18" s="79">
         <v>0.19</v>
-      </c>
-      <c r="K18" s="78">
-        <v>0.15</v>
-      </c>
-      <c r="L18" s="79">
-        <v>0.17</v>
       </c>
       <c r="M18" s="94">
         <v>59.99</v>
@@ -2404,7 +2355,7 @@
         <v>64.97</v>
       </c>
       <c r="P18" s="79">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q18" s="42">
         <v>0</v>
@@ -2418,37 +2369,37 @@
         <v>28</v>
       </c>
       <c r="B19" s="30">
-        <v>1163</v>
+        <v>1122</v>
       </c>
       <c r="C19" s="31">
-        <v>1019</v>
+        <v>982</v>
       </c>
       <c r="D19" s="32">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="E19" s="32">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="F19" s="33">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="G19" s="84">
-        <v>0.20505809979494191</v>
+        <v>0.23255813953488372</v>
       </c>
       <c r="H19" s="85">
-        <v>0.21251931993817619</v>
+        <v>0.24111282843894899</v>
       </c>
       <c r="I19" s="94">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="J19" s="95">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="K19" s="78">
+        <v>0.19</v>
+      </c>
+      <c r="L19" s="79">
         <v>0.17</v>
-      </c>
-      <c r="L19" s="79">
-        <v>0.15</v>
       </c>
       <c r="M19" s="94">
         <v>59.99</v>
@@ -2457,10 +2408,10 @@
         <v>59.99</v>
       </c>
       <c r="O19" s="78">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P19" s="79">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q19" s="42">
         <v>0</v>
@@ -2474,37 +2425,37 @@
         <v>29</v>
       </c>
       <c r="B20" s="30">
-        <v>1436</v>
+        <v>1413</v>
       </c>
       <c r="C20" s="31">
-        <v>1053</v>
+        <v>1014</v>
       </c>
       <c r="D20" s="32">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="E20" s="32">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="F20" s="33">
-        <v>3121</v>
+        <v>3122</v>
       </c>
       <c r="G20" s="84">
-        <v>0.19506726457399104</v>
+        <v>0.20840336134453782</v>
       </c>
       <c r="H20" s="85">
-        <v>0.21241585639491398</v>
+        <v>0.24158563949139866</v>
       </c>
       <c r="I20" s="94">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="J20" s="95">
+        <v>0.17</v>
+      </c>
+      <c r="K20" s="78">
+        <v>0.21</v>
+      </c>
+      <c r="L20" s="79">
         <v>0.18</v>
-      </c>
-      <c r="K20" s="78">
-        <v>0.19</v>
-      </c>
-      <c r="L20" s="79">
-        <v>0.16</v>
       </c>
       <c r="M20" s="94">
         <v>59.99</v>
@@ -2516,7 +2467,7 @@
         <v>64.959999999999994</v>
       </c>
       <c r="P20" s="79">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q20" s="42">
         <v>0</v>
@@ -2530,37 +2481,37 @@
         <v>30</v>
       </c>
       <c r="B21" s="30">
-        <v>2031</v>
+        <v>1897</v>
       </c>
       <c r="C21" s="31">
-        <v>982</v>
+        <v>928</v>
       </c>
       <c r="D21" s="32">
-        <v>572</v>
+        <v>707</v>
       </c>
       <c r="E21" s="32">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="F21" s="33">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="G21" s="84">
-        <v>0.21974644640799079</v>
+        <v>0.271505376344086</v>
       </c>
       <c r="H21" s="85">
-        <v>0.28737300435413643</v>
+        <v>0.32656023222060959</v>
       </c>
       <c r="I21" s="94">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="J21" s="95">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="K21" s="78">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="L21" s="79">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="M21" s="94">
         <v>59.98</v>
@@ -2569,10 +2520,10 @@
         <v>59.99</v>
       </c>
       <c r="O21" s="78">
-        <v>64.930000000000007</v>
+        <v>64.91</v>
       </c>
       <c r="P21" s="79">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q21" s="42">
         <v>0.23</v>
@@ -2586,37 +2537,37 @@
         <v>31</v>
       </c>
       <c r="B22" s="45">
-        <v>2635</v>
+        <v>2477</v>
       </c>
       <c r="C22" s="46">
-        <v>983</v>
+        <v>929</v>
       </c>
       <c r="D22" s="47">
-        <v>743</v>
+        <v>902</v>
       </c>
       <c r="E22" s="47">
-        <v>397</v>
+        <v>450</v>
       </c>
       <c r="F22" s="48">
         <v>4758</v>
       </c>
       <c r="G22" s="86">
-        <v>0.21995263469508586</v>
+        <v>0.26694288250961823</v>
       </c>
       <c r="H22" s="87">
-        <v>0.28768115942028988</v>
+        <v>0.32632342277012327</v>
       </c>
       <c r="I22" s="96">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="J22" s="97">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="K22" s="80">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="L22" s="81">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="M22" s="96">
         <v>59.97</v>
@@ -2625,10 +2576,10 @@
         <v>59.99</v>
       </c>
       <c r="O22" s="80">
-        <v>64.900000000000006</v>
+        <v>64.86</v>
       </c>
       <c r="P22" s="81">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q22" s="53">
         <v>0.23</v>
@@ -2642,37 +2593,37 @@
         <v>32</v>
       </c>
       <c r="B23" s="45">
-        <v>2614</v>
+        <v>2456</v>
       </c>
       <c r="C23" s="46">
-        <v>1027</v>
+        <v>991</v>
       </c>
       <c r="D23" s="47">
-        <v>737</v>
+        <v>896</v>
       </c>
       <c r="E23" s="47">
-        <v>414</v>
+        <v>450</v>
       </c>
       <c r="F23" s="48">
-        <v>4792</v>
+        <v>4793</v>
       </c>
       <c r="G23" s="86">
-        <v>0.21993434795583408</v>
+        <v>0.26730310262529833</v>
       </c>
       <c r="H23" s="87">
-        <v>0.28730048577376821</v>
+        <v>0.31228313671061764</v>
       </c>
       <c r="I23" s="96">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
       <c r="J23" s="97">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="K23" s="80">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="L23" s="81">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="M23" s="96">
         <v>59.97</v>
@@ -2681,7 +2632,7 @@
         <v>59.99</v>
       </c>
       <c r="O23" s="80">
-        <v>64.900000000000006</v>
+        <v>64.86</v>
       </c>
       <c r="P23" s="81">
         <v>64.95</v>
@@ -2698,37 +2649,37 @@
         <v>33</v>
       </c>
       <c r="B24" s="45">
-        <v>2032</v>
+        <v>1897</v>
       </c>
       <c r="C24" s="46">
-        <v>865</v>
+        <v>790</v>
       </c>
       <c r="D24" s="47">
-        <v>572</v>
+        <v>708</v>
       </c>
       <c r="E24" s="47">
-        <v>349</v>
+        <v>424</v>
       </c>
       <c r="F24" s="48">
-        <v>3818</v>
+        <v>3819</v>
       </c>
       <c r="G24" s="86">
-        <v>0.2196620583717358</v>
+        <v>0.27178502879078698</v>
       </c>
       <c r="H24" s="87">
-        <v>0.28747940691927515</v>
+        <v>0.34925864909390447</v>
       </c>
       <c r="I24" s="96">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="J24" s="97">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K24" s="80">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="L24" s="81">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="M24" s="96">
         <v>59.98</v>
@@ -2737,10 +2688,10 @@
         <v>59.99</v>
       </c>
       <c r="O24" s="80">
-        <v>64.930000000000007</v>
+        <v>64.91</v>
       </c>
       <c r="P24" s="81">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q24" s="53">
         <v>0.23</v>
@@ -2754,25 +2705,25 @@
         <v>34</v>
       </c>
       <c r="B25" s="30">
-        <v>1390</v>
+        <v>1374</v>
       </c>
       <c r="C25" s="31">
-        <v>638</v>
+        <v>615</v>
       </c>
       <c r="D25" s="32">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="E25" s="32">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="F25" s="33">
         <v>2546</v>
       </c>
       <c r="G25" s="84">
-        <v>0.19930875576036866</v>
+        <v>0.20852534562211983</v>
       </c>
       <c r="H25" s="85">
-        <v>0.21234567901234569</v>
+        <v>0.24074074074074073</v>
       </c>
       <c r="I25" s="94">
         <v>0.24</v>
@@ -2781,10 +2732,10 @@
         <v>0.11</v>
       </c>
       <c r="K25" s="78">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="L25" s="79">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="M25" s="94">
         <v>59.99</v>
@@ -2810,37 +2761,37 @@
         <v>35</v>
       </c>
       <c r="B26" s="30">
-        <v>994</v>
+        <v>959</v>
       </c>
       <c r="C26" s="31">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D26" s="32">
-        <v>255</v>
+        <v>290</v>
       </c>
       <c r="E26" s="32">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="F26" s="33">
         <v>1781</v>
       </c>
       <c r="G26" s="84">
-        <v>0.20416333066453163</v>
+        <v>0.23218574859887911</v>
       </c>
       <c r="H26" s="85">
-        <v>0.21240601503759399</v>
+        <v>0.24060150375939848</v>
       </c>
       <c r="I26" s="94">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J26" s="95">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K26" s="78">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="L26" s="79">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M26" s="94">
         <v>59.99</v>
@@ -2866,25 +2817,25 @@
         <v>36</v>
       </c>
       <c r="B27" s="30">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="C27" s="31">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D27" s="32">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E27" s="32">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F27" s="33">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="G27" s="84">
-        <v>0.1521099116781158</v>
+        <v>0.15815324165029471</v>
       </c>
       <c r="H27" s="85">
-        <v>0.15827338129496402</v>
+        <v>0.16306954436450841</v>
       </c>
       <c r="I27" s="94">
         <v>0.15</v>
@@ -2908,7 +2859,7 @@
         <v>64.98</v>
       </c>
       <c r="P27" s="79">
-        <v>64.989999999999995</v>
+        <v>64.98</v>
       </c>
       <c r="Q27" s="42">
         <v>0</v>
@@ -2922,25 +2873,25 @@
         <v>37</v>
       </c>
       <c r="B28" s="30">
-        <v>685</v>
+        <v>700</v>
       </c>
       <c r="C28" s="31">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D28" s="32">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E28" s="32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F28" s="33">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="G28" s="84">
-        <v>7.307171853856563E-2</v>
+        <v>5.2774018944519621E-2</v>
       </c>
       <c r="H28" s="85">
-        <v>7.4204946996466431E-2</v>
+        <v>5.6338028169014086E-2</v>
       </c>
       <c r="I28" s="94">
         <v>0.12</v>
@@ -2949,7 +2900,7 @@
         <v>0.05</v>
       </c>
       <c r="K28" s="78">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="L28" s="79">
         <v>0.01</v>
@@ -2978,28 +2929,28 @@
         <v>38</v>
       </c>
       <c r="B29" s="55">
-        <v>493</v>
+        <v>503</v>
       </c>
       <c r="C29" s="56">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D29" s="57">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E29" s="57">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" s="58">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G29" s="88">
-        <v>7.3308270676691725E-2</v>
+        <v>5.2730696798493411E-2</v>
       </c>
       <c r="H29" s="89">
-        <v>7.5949367088607597E-2</v>
+        <v>5.6962025316455694E-2</v>
       </c>
       <c r="I29" s="98">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="J29" s="99">
         <v>0.03</v>
@@ -3008,7 +2959,7 @@
         <v>0.02</v>
       </c>
       <c r="L29" s="83">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M29" s="98">
         <v>59.99</v>
@@ -3035,31 +2986,31 @@
       </c>
       <c r="B30" s="65">
         <f>SUM(B6:B29)</f>
-        <v>22579</v>
+        <v>21609</v>
       </c>
       <c r="C30" s="66">
         <f t="shared" ref="C30:F30" si="0">SUM(C6:C29)</f>
-        <v>21979</v>
+        <v>20920</v>
       </c>
       <c r="D30" s="67">
         <f t="shared" si="0"/>
-        <v>5934</v>
+        <v>6906</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" si="0"/>
-        <v>6531</v>
+        <v>7592</v>
       </c>
       <c r="F30" s="68">
         <f t="shared" si="0"/>
-        <v>57023</v>
+        <v>57027</v>
       </c>
       <c r="G30" s="100">
         <f>D30/B30</f>
-        <v>0.26281057619912307</v>
+        <v>0.31958906011384147</v>
       </c>
       <c r="H30" s="101">
         <f>E30/C30</f>
-        <v>0.29714727694617588</v>
+        <v>0.36290630975143401</v>
       </c>
       <c r="I30" s="71"/>
       <c r="J30" s="71"/>
@@ -3072,7 +3023,7 @@
       </c>
       <c r="B32" s="72">
         <f>B30+C30</f>
-        <v>44558</v>
+        <v>42529</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -3081,7 +3032,7 @@
       </c>
       <c r="B33" s="72">
         <f>D30+E30</f>
-        <v>12465</v>
+        <v>14498</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3090,7 +3041,7 @@
       </c>
       <c r="B34" s="72">
         <f>B32+B33</f>
-        <v>57023</v>
+        <v>57027</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3391,31 +3342,31 @@
         <v>15</v>
       </c>
       <c r="B51" s="30">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C51" s="31">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D51" s="32">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E51" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F51" s="33">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G51" s="84">
-        <v>7.7669902912621352E-2</v>
+        <v>5.8252427184466021E-2</v>
       </c>
       <c r="H51" s="85">
-        <v>6.4516129032258063E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="I51" s="90">
         <v>0.05</v>
       </c>
       <c r="J51" s="91">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K51" s="92">
         <v>0.01</v>
@@ -3447,25 +3398,25 @@
         <v>16</v>
       </c>
       <c r="B52" s="30">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C52" s="31">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D52" s="32">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E52" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" s="33">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G52" s="84">
-        <v>7.6023391812865493E-2</v>
+        <v>5.8139534883720929E-2</v>
       </c>
       <c r="H52" s="85">
-        <v>5.9701492537313432E-2</v>
+        <v>4.4776119402985072E-2</v>
       </c>
       <c r="I52" s="94">
         <v>0.03</v>
@@ -3503,25 +3454,25 @@
         <v>17</v>
       </c>
       <c r="B53" s="30">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C53" s="31">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D53" s="32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E53" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" s="33">
         <v>178</v>
       </c>
       <c r="G53" s="84">
-        <v>7.7586206896551727E-2</v>
+        <v>6.0344827586206899E-2</v>
       </c>
       <c r="H53" s="85">
-        <v>6.4516129032258063E-2</v>
+        <v>4.8387096774193547E-2</v>
       </c>
       <c r="I53" s="94">
         <v>0.02</v>
@@ -3559,25 +3510,25 @@
         <v>18</v>
       </c>
       <c r="B54" s="30">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C54" s="31">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D54" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E54" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F54" s="33">
         <v>233</v>
       </c>
       <c r="G54" s="84">
-        <v>7.476635514018691E-2</v>
+        <v>5.6074766355140186E-2</v>
       </c>
       <c r="H54" s="85">
-        <v>6.3492063492063489E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="I54" s="94">
         <v>0.02</v>
@@ -3615,25 +3566,25 @@
         <v>19</v>
       </c>
       <c r="B55" s="30">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C55" s="31">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D55" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E55" s="32">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F55" s="33">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G55" s="84">
-        <v>7.4829931972789115E-2</v>
+        <v>5.4421768707482991E-2</v>
       </c>
       <c r="H55" s="85">
-        <v>6.0344827586206899E-2</v>
+        <v>4.3227665706051875E-2</v>
       </c>
       <c r="I55" s="94">
         <v>0.02</v>
@@ -3642,7 +3593,7 @@
         <v>0.06</v>
       </c>
       <c r="K55" s="78">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L55" s="79">
         <v>0.01</v>
@@ -3671,25 +3622,25 @@
         <v>20</v>
       </c>
       <c r="B56" s="30">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C56" s="31">
-        <v>1112</v>
+        <v>1105</v>
       </c>
       <c r="D56" s="32">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E56" s="32">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="F56" s="33">
         <v>1555</v>
       </c>
       <c r="G56" s="84">
-        <v>0.16071428571428573</v>
+        <v>0.16785714285714284</v>
       </c>
       <c r="H56" s="85">
-        <v>0.12784313725490196</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I56" s="94">
         <v>0.04</v>
@@ -3727,49 +3678,49 @@
         <v>21</v>
       </c>
       <c r="B57" s="30">
-        <v>539</v>
+        <v>491</v>
       </c>
       <c r="C57" s="31">
-        <v>3182</v>
+        <v>3017</v>
       </c>
       <c r="D57" s="32">
-        <v>225</v>
+        <v>273</v>
       </c>
       <c r="E57" s="32">
-        <v>758</v>
+        <v>923</v>
       </c>
       <c r="F57" s="33">
         <v>4704</v>
       </c>
       <c r="G57" s="84">
-        <v>0.29450261780104714</v>
+        <v>0.35732984293193715</v>
       </c>
       <c r="H57" s="85">
-        <v>0.19238578680203045</v>
+        <v>0.23426395939086295</v>
       </c>
       <c r="I57" s="94">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="J57" s="95">
-        <v>0.55000000000000004</v>
+        <v>0.52</v>
       </c>
       <c r="K57" s="78">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="L57" s="79">
-        <v>0.42</v>
+        <v>0.51</v>
       </c>
       <c r="M57" s="94">
         <v>59.99</v>
       </c>
       <c r="N57" s="95">
-        <v>59.95</v>
+        <v>59.96</v>
       </c>
       <c r="O57" s="78">
         <v>64.97</v>
       </c>
       <c r="P57" s="79">
-        <v>64.900000000000006</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="Q57" s="42">
         <v>0</v>
@@ -3783,49 +3734,49 @@
         <v>22</v>
       </c>
       <c r="B58" s="45">
-        <v>849</v>
+        <v>774</v>
       </c>
       <c r="C58" s="46">
-        <v>3319</v>
+        <v>3160</v>
       </c>
       <c r="D58" s="47">
-        <v>355</v>
+        <v>430</v>
       </c>
       <c r="E58" s="47">
-        <v>824</v>
+        <v>983</v>
       </c>
       <c r="F58" s="48">
         <v>5347</v>
       </c>
       <c r="G58" s="86">
-        <v>0.29485049833887045</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="H58" s="87">
-        <v>0.19888969345884625</v>
+        <v>0.23726768042481294</v>
       </c>
       <c r="I58" s="96">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="J58" s="97">
-        <v>0.56999999999999995</v>
+        <v>0.54</v>
       </c>
       <c r="K58" s="80">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="L58" s="81">
-        <v>0.46</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M58" s="96">
         <v>59.99</v>
       </c>
       <c r="N58" s="97">
-        <v>59.95</v>
+        <v>59.96</v>
       </c>
       <c r="O58" s="80">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="P58" s="81">
-        <v>64.88</v>
+        <v>64.83</v>
       </c>
       <c r="Q58" s="53">
         <v>0</v>
@@ -3839,37 +3790,37 @@
         <v>23</v>
       </c>
       <c r="B59" s="45">
-        <v>879</v>
+        <v>802</v>
       </c>
       <c r="C59" s="46">
-        <v>3095</v>
+        <v>2930</v>
       </c>
       <c r="D59" s="47">
-        <v>367</v>
+        <v>445</v>
       </c>
       <c r="E59" s="47">
-        <v>729</v>
+        <v>894</v>
       </c>
       <c r="F59" s="48">
-        <v>5070</v>
+        <v>5071</v>
       </c>
       <c r="G59" s="86">
-        <v>0.2945425361155698</v>
+        <v>0.35685645549318362</v>
       </c>
       <c r="H59" s="87">
-        <v>0.19063807531380753</v>
+        <v>0.23378661087866109</v>
       </c>
       <c r="I59" s="96">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J59" s="97">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
       <c r="K59" s="80">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="L59" s="81">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="M59" s="96">
         <v>59.99</v>
@@ -3878,10 +3829,10 @@
         <v>59.96</v>
       </c>
       <c r="O59" s="80">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="P59" s="81">
-        <v>64.900000000000006</v>
+        <v>64.86</v>
       </c>
       <c r="Q59" s="53">
         <v>0</v>
@@ -3895,37 +3846,37 @@
         <v>24</v>
       </c>
       <c r="B60" s="45">
-        <v>922</v>
+        <v>857</v>
       </c>
       <c r="C60" s="46">
-        <v>2171</v>
+        <v>2068</v>
       </c>
       <c r="D60" s="47">
-        <v>385</v>
+        <v>450</v>
       </c>
       <c r="E60" s="47">
-        <v>521</v>
+        <v>624</v>
       </c>
       <c r="F60" s="48">
         <v>3999</v>
       </c>
       <c r="G60" s="86">
-        <v>0.29456771231828616</v>
+        <v>0.34429992348890587</v>
       </c>
       <c r="H60" s="87">
-        <v>0.19353640416047549</v>
+        <v>0.23179791976225855</v>
       </c>
       <c r="I60" s="96">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="J60" s="97">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="K60" s="80">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
       <c r="L60" s="81">
-        <v>0.28999999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="M60" s="96">
         <v>59.99</v>
@@ -3934,16 +3885,16 @@
         <v>59.98</v>
       </c>
       <c r="O60" s="80">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="P60" s="81">
-        <v>64.94</v>
+        <v>64.92</v>
       </c>
       <c r="Q60" s="53">
         <v>0</v>
       </c>
       <c r="R60" s="54">
-        <v>0</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3951,37 +3902,37 @@
         <v>25</v>
       </c>
       <c r="B61" s="30">
-        <v>987</v>
+        <v>949</v>
       </c>
       <c r="C61" s="31">
-        <v>1737</v>
+        <v>1688</v>
       </c>
       <c r="D61" s="32">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="E61" s="32">
-        <v>363</v>
+        <v>413</v>
       </c>
       <c r="F61" s="33">
         <v>3363</v>
       </c>
       <c r="G61" s="84">
-        <v>0.21852731591448932</v>
+        <v>0.24801901743264659</v>
       </c>
       <c r="H61" s="85">
-        <v>0.17285714285714285</v>
+        <v>0.196573060447406</v>
       </c>
       <c r="I61" s="94">
+        <v>0.16</v>
+      </c>
+      <c r="J61" s="95">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K61" s="78">
         <v>0.17</v>
       </c>
-      <c r="J61" s="95">
-        <v>0.3</v>
-      </c>
-      <c r="K61" s="78">
-        <v>0.15</v>
-      </c>
       <c r="L61" s="79">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="M61" s="94">
         <v>59.99</v>
@@ -3990,10 +3941,10 @@
         <v>59.98</v>
       </c>
       <c r="O61" s="78">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P61" s="79">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q61" s="42">
         <v>0</v>
@@ -4007,25 +3958,25 @@
         <v>26</v>
       </c>
       <c r="B62" s="30">
-        <v>1076</v>
+        <v>1035</v>
       </c>
       <c r="C62" s="31">
-        <v>1542</v>
+        <v>1498</v>
       </c>
       <c r="D62" s="32">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="E62" s="32">
-        <v>322</v>
+        <v>366</v>
       </c>
       <c r="F62" s="33">
-        <v>3241</v>
+        <v>3240</v>
       </c>
       <c r="G62" s="84">
-        <v>0.21859114015976761</v>
+        <v>0.24781976744186046</v>
       </c>
       <c r="H62" s="85">
-        <v>0.17274678111587982</v>
+        <v>0.1963519313304721</v>
       </c>
       <c r="I62" s="94">
         <v>0.18</v>
@@ -4034,10 +3985,10 @@
         <v>0.26</v>
       </c>
       <c r="K62" s="78">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="L62" s="79">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="M62" s="94">
         <v>59.99</v>
@@ -4046,7 +3997,7 @@
         <v>59.99</v>
       </c>
       <c r="O62" s="78">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="P62" s="79">
         <v>64.959999999999994</v>
@@ -4063,25 +4014,25 @@
         <v>27</v>
       </c>
       <c r="B63" s="30">
-        <v>1244</v>
+        <v>1196</v>
       </c>
       <c r="C63" s="31">
-        <v>1410</v>
+        <v>1369</v>
       </c>
       <c r="D63" s="32">
-        <v>347</v>
+        <v>394</v>
       </c>
       <c r="E63" s="32">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="F63" s="33">
-        <v>3295</v>
+        <v>3294</v>
       </c>
       <c r="G63" s="84">
-        <v>0.21810182275298554</v>
+        <v>0.24779874213836478</v>
       </c>
       <c r="H63" s="85">
-        <v>0.17253521126760563</v>
+        <v>0.19659624413145541</v>
       </c>
       <c r="I63" s="94">
         <v>0.21</v>
@@ -4090,10 +4041,10 @@
         <v>0.24</v>
       </c>
       <c r="K63" s="78">
+        <v>0.22</v>
+      </c>
+      <c r="L63" s="79">
         <v>0.19</v>
-      </c>
-      <c r="L63" s="79">
-        <v>0.16</v>
       </c>
       <c r="M63" s="94">
         <v>59.99</v>
@@ -4105,7 +4056,7 @@
         <v>64.959999999999994</v>
       </c>
       <c r="P63" s="79">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q63" s="42">
         <v>0</v>
@@ -4119,37 +4070,37 @@
         <v>28</v>
       </c>
       <c r="B64" s="30">
-        <v>1403</v>
+        <v>1349</v>
       </c>
       <c r="C64" s="31">
-        <v>1303</v>
+        <v>1266</v>
       </c>
       <c r="D64" s="32">
-        <v>392</v>
+        <v>445</v>
       </c>
       <c r="E64" s="32">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="F64" s="33">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="G64" s="84">
-        <v>0.21838440111420612</v>
+        <v>0.24804905239687849</v>
       </c>
       <c r="H64" s="85">
-        <v>0.17269841269841271</v>
+        <v>0.19619047619047619</v>
       </c>
       <c r="I64" s="94">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="J64" s="95">
         <v>0.22</v>
       </c>
       <c r="K64" s="78">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="L64" s="79">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="M64" s="94">
         <v>59.99</v>
@@ -4158,10 +4109,10 @@
         <v>59.99</v>
       </c>
       <c r="O64" s="78">
+        <v>64.95</v>
+      </c>
+      <c r="P64" s="79">
         <v>64.959999999999994</v>
-      </c>
-      <c r="P64" s="79">
-        <v>64.97</v>
       </c>
       <c r="Q64" s="42">
         <v>0</v>
@@ -4175,37 +4126,37 @@
         <v>29</v>
       </c>
       <c r="B65" s="30">
-        <v>1739</v>
+        <v>1715</v>
       </c>
       <c r="C65" s="31">
-        <v>1346</v>
+        <v>1308</v>
       </c>
       <c r="D65" s="32">
-        <v>450</v>
+        <v>474</v>
       </c>
       <c r="E65" s="32">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="F65" s="33">
-        <v>3816</v>
+        <v>3817</v>
       </c>
       <c r="G65" s="84">
-        <v>0.2055733211512106</v>
+        <v>0.21653723161260849</v>
       </c>
       <c r="H65" s="85">
-        <v>0.17271051014136449</v>
+        <v>0.19656019656019655</v>
       </c>
       <c r="I65" s="94">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J65" s="95">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="K65" s="78">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="L65" s="79">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="M65" s="94">
         <v>59.98</v>
@@ -4217,7 +4168,7 @@
         <v>64.95</v>
       </c>
       <c r="P65" s="79">
-        <v>64.97</v>
+        <v>64.959999999999994</v>
       </c>
       <c r="Q65" s="42">
         <v>0</v>
@@ -4231,49 +4182,49 @@
         <v>30</v>
       </c>
       <c r="B66" s="30">
-        <v>2426</v>
+        <v>2250</v>
       </c>
       <c r="C66" s="31">
-        <v>1285</v>
+        <v>1228</v>
       </c>
       <c r="D66" s="32">
-        <v>767</v>
+        <v>943</v>
       </c>
       <c r="E66" s="32">
-        <v>393</v>
+        <v>450</v>
       </c>
       <c r="F66" s="33">
         <v>4871</v>
       </c>
       <c r="G66" s="84">
-        <v>0.24021296586282492</v>
+        <v>0.29533354212339491</v>
       </c>
       <c r="H66" s="85">
-        <v>0.23420738974970204</v>
+        <v>0.26817640047675806</v>
       </c>
       <c r="I66" s="94">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="J66" s="95">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="K66" s="78">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
       <c r="L66" s="79">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="M66" s="94">
-        <v>59.97</v>
+        <v>59.98</v>
       </c>
       <c r="N66" s="95">
         <v>59.99</v>
       </c>
       <c r="O66" s="78">
-        <v>64.900000000000006</v>
+        <v>64.84</v>
       </c>
       <c r="P66" s="79">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q66" s="42">
         <v>0.23</v>
@@ -4287,37 +4238,37 @@
         <v>31</v>
       </c>
       <c r="B67" s="45">
-        <v>3147</v>
+        <v>2952</v>
       </c>
       <c r="C67" s="46">
-        <v>1286</v>
+        <v>1229</v>
       </c>
       <c r="D67" s="47">
-        <v>997</v>
+        <v>1192</v>
       </c>
       <c r="E67" s="47">
-        <v>393</v>
+        <v>450</v>
       </c>
       <c r="F67" s="48">
         <v>5823</v>
       </c>
       <c r="G67" s="86">
-        <v>0.24058880308880309</v>
+        <v>0.28764478764478763</v>
       </c>
       <c r="H67" s="87">
-        <v>0.23406789755807028</v>
+        <v>0.26801667659321027</v>
       </c>
       <c r="I67" s="96">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="J67" s="97">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="K67" s="80">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L67" s="81">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="M67" s="96">
         <v>59.96</v>
@@ -4326,13 +4277,13 @@
         <v>59.99</v>
       </c>
       <c r="O67" s="80">
-        <v>64.819999999999993</v>
+        <v>64.7</v>
       </c>
       <c r="P67" s="81">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q67" s="53">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="R67" s="54">
         <v>0</v>
@@ -4343,37 +4294,37 @@
         <v>32</v>
       </c>
       <c r="B68" s="45">
-        <v>3122</v>
+        <v>2927</v>
       </c>
       <c r="C68" s="46">
-        <v>1344</v>
+        <v>1305</v>
       </c>
       <c r="D68" s="47">
-        <v>989</v>
+        <v>1184</v>
       </c>
       <c r="E68" s="47">
-        <v>411</v>
+        <v>450</v>
       </c>
       <c r="F68" s="48">
         <v>5866</v>
       </c>
       <c r="G68" s="86">
-        <v>0.24057406956944782</v>
+        <v>0.28800778399416199</v>
       </c>
       <c r="H68" s="87">
-        <v>0.23418803418803419</v>
+        <v>0.25641025641025639</v>
       </c>
       <c r="I68" s="96">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="J68" s="97">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="K68" s="80">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L68" s="81">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="M68" s="96">
         <v>59.96</v>
@@ -4382,13 +4333,13 @@
         <v>59.99</v>
       </c>
       <c r="O68" s="80">
-        <v>64.83</v>
+        <v>64.709999999999994</v>
       </c>
       <c r="P68" s="81">
         <v>64.95</v>
       </c>
       <c r="Q68" s="53">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="R68" s="54">
         <v>0</v>
@@ -4399,49 +4350,49 @@
         <v>33</v>
       </c>
       <c r="B69" s="45">
-        <v>2427</v>
+        <v>2250</v>
       </c>
       <c r="C69" s="46">
-        <v>1131</v>
+        <v>1057</v>
       </c>
       <c r="D69" s="47">
-        <v>768</v>
+        <v>945</v>
       </c>
       <c r="E69" s="47">
-        <v>346</v>
+        <v>420</v>
       </c>
       <c r="F69" s="48">
         <v>4672</v>
       </c>
       <c r="G69" s="86">
-        <v>0.24037558685446009</v>
+        <v>0.29577464788732394</v>
       </c>
       <c r="H69" s="87">
-        <v>0.23425863236289776</v>
+        <v>0.28436018957345971</v>
       </c>
       <c r="I69" s="96">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="J69" s="97">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="K69" s="80">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
       <c r="L69" s="81">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
       <c r="M69" s="96">
-        <v>59.97</v>
+        <v>59.98</v>
       </c>
       <c r="N69" s="97">
         <v>59.99</v>
       </c>
       <c r="O69" s="80">
-        <v>64.900000000000006</v>
+        <v>64.84</v>
       </c>
       <c r="P69" s="81">
-        <v>64.959999999999994</v>
+        <v>64.95</v>
       </c>
       <c r="Q69" s="53">
         <v>0.23</v>
@@ -4455,25 +4406,25 @@
         <v>34</v>
       </c>
       <c r="B70" s="30">
-        <v>1680</v>
+        <v>1668</v>
       </c>
       <c r="C70" s="31">
-        <v>816</v>
+        <v>793</v>
       </c>
       <c r="D70" s="32">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="E70" s="32">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="F70" s="33">
-        <v>3116</v>
+        <v>3117</v>
       </c>
       <c r="G70" s="84">
-        <v>0.21126760563380281</v>
+        <v>0.21690140845070421</v>
       </c>
       <c r="H70" s="85">
-        <v>0.17241379310344829</v>
+        <v>0.19655521783181357</v>
       </c>
       <c r="I70" s="94">
         <v>0.28999999999999998</v>
@@ -4482,10 +4433,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="K70" s="78">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="L70" s="79">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="M70" s="94">
         <v>59.98</v>
@@ -4511,37 +4462,37 @@
         <v>35</v>
       </c>
       <c r="B71" s="30">
-        <v>1198</v>
+        <v>1153</v>
       </c>
       <c r="C71" s="31">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="D71" s="32">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="E71" s="32">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="F71" s="33">
         <v>2180</v>
       </c>
       <c r="G71" s="84">
-        <v>0.21801566579634465</v>
+        <v>0.24738903394255873</v>
       </c>
       <c r="H71" s="85">
-        <v>0.1728395061728395</v>
+        <v>0.19598765432098766</v>
       </c>
       <c r="I71" s="94">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="J71" s="95">
         <v>0.09</v>
       </c>
       <c r="K71" s="78">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="L71" s="79">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M71" s="94">
         <v>59.99</v>
@@ -4567,25 +4518,25 @@
         <v>36</v>
       </c>
       <c r="B72" s="30">
-        <v>1047</v>
+        <v>1038</v>
       </c>
       <c r="C72" s="31">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D72" s="32">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E72" s="32">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F72" s="33">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="G72" s="84">
-        <v>0.16239999999999999</v>
+        <v>0.1689351481184948</v>
       </c>
       <c r="H72" s="85">
-        <v>0.12795275590551181</v>
+        <v>0.13385826771653545</v>
       </c>
       <c r="I72" s="94">
         <v>0.18</v>
@@ -4594,7 +4545,7 @@
         <v>0.08</v>
       </c>
       <c r="K72" s="78">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="L72" s="79">
         <v>0.04</v>
@@ -4623,34 +4574,34 @@
         <v>37</v>
       </c>
       <c r="B73" s="30">
-        <v>836</v>
+        <v>855</v>
       </c>
       <c r="C73" s="31">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="D73" s="32">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="E73" s="32">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F73" s="33">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="G73" s="84">
-        <v>7.7262693156732898E-2</v>
+        <v>5.6291390728476824E-2</v>
       </c>
       <c r="H73" s="85">
-        <v>6.0869565217391307E-2</v>
+        <v>4.3604651162790699E-2</v>
       </c>
       <c r="I73" s="94">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J73" s="95">
         <v>0.06</v>
       </c>
       <c r="K73" s="78">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="L73" s="79">
         <v>0.01</v>
@@ -4662,7 +4613,7 @@
         <v>60</v>
       </c>
       <c r="O73" s="78">
-        <v>64.98</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="P73" s="79">
         <v>64.989999999999995</v>
@@ -4679,37 +4630,37 @@
         <v>38</v>
       </c>
       <c r="B74" s="55">
-        <v>601</v>
+        <v>615</v>
       </c>
       <c r="C74" s="56">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D74" s="57">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E74" s="57">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F74" s="58">
         <v>844</v>
       </c>
       <c r="G74" s="88">
-        <v>7.8220858895705528E-2</v>
+        <v>5.674846625766871E-2</v>
       </c>
       <c r="H74" s="89">
-        <v>6.25E-2</v>
+        <v>4.6875E-2</v>
       </c>
       <c r="I74" s="98">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J74" s="99">
         <v>0.03</v>
       </c>
       <c r="K74" s="82">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="L74" s="83">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M74" s="98">
         <v>59.99</v>
@@ -4736,31 +4687,31 @@
       </c>
       <c r="B75" s="65">
         <f>SUM(B51:B74)</f>
-        <v>27142</v>
+        <v>25911</v>
       </c>
       <c r="C75" s="66">
         <f t="shared" ref="C75" si="1">SUM(C51:C74)</f>
-        <v>28215</v>
+        <v>27157</v>
       </c>
       <c r="D75" s="67">
         <f t="shared" ref="D75" si="2">SUM(D51:D74)</f>
-        <v>7837</v>
+        <v>9065</v>
       </c>
       <c r="E75" s="67">
         <f t="shared" ref="E75" si="3">SUM(E51:E74)</f>
-        <v>6493</v>
+        <v>7551</v>
       </c>
       <c r="F75" s="68">
         <f t="shared" ref="F75" si="4">SUM(F51:F74)</f>
-        <v>69687</v>
+        <v>69684</v>
       </c>
       <c r="G75" s="100">
         <f>D75/B75</f>
-        <v>0.28874069707464445</v>
+        <v>0.34985141445718032</v>
       </c>
       <c r="H75" s="101">
         <f>E75/C75</f>
-        <v>0.23012581959950382</v>
+        <v>0.27804985823176342</v>
       </c>
       <c r="I75" s="71"/>
       <c r="J75" s="71"/>
@@ -4773,7 +4724,7 @@
       </c>
       <c r="B77" s="72">
         <f>B75+C75</f>
-        <v>55357</v>
+        <v>53068</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -4782,7 +4733,7 @@
       </c>
       <c r="B78" s="72">
         <f>D75+E75</f>
-        <v>14330</v>
+        <v>16616</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -4791,7 +4742,7 @@
       </c>
       <c r="B79" s="72">
         <f>B77+B78</f>
-        <v>69687</v>
+        <v>69684</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -15371,6 +15322,5 @@
     <mergeCell ref="Q723:R723"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>